<commit_message>
add calculations and dimensions
</commit_message>
<xml_diff>
--- a/GraduationCapDesign_2017.xlsx
+++ b/GraduationCapDesign_2017.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>LED count</t>
   </si>
@@ -59,13 +59,74 @@
   </si>
   <si>
     <t>Mokungit 93 Leds WS2812B WS2812 5050 RGB LED Ring Lamp Light with Integrated Drivers</t>
+  </si>
+  <si>
+    <t>outside-to-outside outer hole to diag outer hole</t>
+  </si>
+  <si>
+    <t>outside-to-outside outer hole to adjacent outer hole</t>
+  </si>
+  <si>
+    <t>hole diameter</t>
+  </si>
+  <si>
+    <t>rectangle is 85 x 70 mm with 1.5 mm holes</t>
+  </si>
+  <si>
+    <t>wide side of rectangle parallel to solder points lineup on adjacent rings</t>
+  </si>
+  <si>
+    <t>mm side of cap</t>
+  </si>
+  <si>
+    <t>mm outside diameter LED ring</t>
+  </si>
+  <si>
+    <t>mm separation between LED rings, both ways</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Cap edge</t>
+  </si>
+  <si>
+    <t>Center LED ring to:</t>
+  </si>
+  <si>
+    <t>center adjacent LED ring</t>
+  </si>
+  <si>
+    <t>Cap edge to:</t>
+  </si>
+  <si>
+    <t>Center LED ring</t>
+  </si>
+  <si>
+    <t>LED ring wide attach</t>
+  </si>
+  <si>
+    <t>LED ring narrow attach</t>
+  </si>
+  <si>
+    <t>LED ring wide rectangle</t>
+  </si>
+  <si>
+    <t>LED ring narrow rectangle</t>
+  </si>
+  <si>
+    <t>angle of diag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +138,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,9 +172,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -232,8 +305,8 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>297873</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
@@ -476,8 +549,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>76952</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>336724</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>162942</xdr:rowOff>
     </xdr:to>
@@ -848,11 +921,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:AC118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB116" sqref="AB116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -953,6 +1032,242 @@
     <row r="18" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q18" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S95" t="s">
+        <v>11</v>
+      </c>
+      <c r="W95" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC95" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S96" s="2">
+        <v>110.66</v>
+      </c>
+      <c r="W96" s="2">
+        <v>85.62</v>
+      </c>
+      <c r="Y96" s="2">
+        <v>70.569999999999993</v>
+      </c>
+      <c r="AC96">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="97" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S97" s="2">
+        <v>110.45</v>
+      </c>
+      <c r="W97" s="2">
+        <v>86.01</v>
+      </c>
+      <c r="Y97" s="2">
+        <v>70.83</v>
+      </c>
+      <c r="AC97">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="98" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S98" s="2">
+        <v>110.61</v>
+      </c>
+      <c r="W98" s="2">
+        <v>85.88</v>
+      </c>
+      <c r="Y98" s="2">
+        <v>70.61</v>
+      </c>
+      <c r="AC98">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="99" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S99" s="2">
+        <v>110.7</v>
+      </c>
+      <c r="W99" s="2">
+        <v>85.6</v>
+      </c>
+      <c r="Y99" s="2">
+        <v>70.69</v>
+      </c>
+      <c r="AC99">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="100" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S100" s="3">
+        <f>AVERAGE(S96:S99)</f>
+        <v>110.605</v>
+      </c>
+      <c r="W100" s="3">
+        <f>AVERAGE(W96:W99)</f>
+        <v>85.777500000000003</v>
+      </c>
+      <c r="Y100" s="3">
+        <f>AVERAGE(Y96:Y99)</f>
+        <v>70.674999999999997</v>
+      </c>
+      <c r="AA100" s="4">
+        <f>SQRT(POWER(W100,2)+POWER(Y100,2))</f>
+        <v>111.14285911047097</v>
+      </c>
+      <c r="AC100" s="3">
+        <f>AVERAGE(AC96:AC99)</f>
+        <v>1.5225</v>
+      </c>
+    </row>
+    <row r="101" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="AA101" s="4"/>
+      <c r="AC101" s="3"/>
+    </row>
+    <row r="102" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S102">
+        <f>S100-0.5*$AC$100</f>
+        <v>109.84375</v>
+      </c>
+      <c r="W102">
+        <f>W100-0.5*$AC$100</f>
+        <v>85.016249999999999</v>
+      </c>
+      <c r="Y102">
+        <f>Y100-0.5*$AC$100</f>
+        <v>69.913749999999993</v>
+      </c>
+      <c r="AA102" s="4">
+        <f t="shared" ref="AA101:AA102" si="0">SQRT(POWER(W102,2)+POWER(Y102,2))</f>
+        <v>110.0713187125738</v>
+      </c>
+    </row>
+    <row r="105" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y105" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y106" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S107">
+        <v>14</v>
+      </c>
+      <c r="T107" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S108">
+        <v>112</v>
+      </c>
+      <c r="T108" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S109">
+        <v>238</v>
+      </c>
+      <c r="T109" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S110">
+        <v>85</v>
+      </c>
+      <c r="T110" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S111">
+        <v>70</v>
+      </c>
+      <c r="T111" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y111" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y112">
+        <f>S108/2</f>
+        <v>56</v>
+      </c>
+      <c r="Z112" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB112">
+        <f>S108/2</f>
+        <v>56</v>
+      </c>
+      <c r="AC112" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y113">
+        <f>S109-S108</f>
+        <v>126</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB113">
+        <f>AB112-S111/2</f>
+        <v>21</v>
+      </c>
+      <c r="AC113" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="S114">
+        <f>2*S108+S107</f>
+        <v>238</v>
+      </c>
+      <c r="T114" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB114">
+        <f>AB112-S110/2</f>
+        <v>13.5</v>
+      </c>
+      <c r="AC114" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="116" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y116" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB116">
+        <f>180/PI()</f>
+        <v>57.295779513082323</v>
+      </c>
+    </row>
+    <row r="117" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y117" s="5">
+        <f>ATAN(S110/S111)*AB116</f>
+        <v>50.527540151656176</v>
+      </c>
+    </row>
+    <row r="118" spans="19:29" x14ac:dyDescent="0.25">
+      <c r="Y118" s="5">
+        <f>ATAN(S111/S110)*AB116</f>
+        <v>39.472459848343824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
information on power and batteries
</commit_message>
<xml_diff>
--- a/GraduationCapDesign_2017.xlsx
+++ b/GraduationCapDesign_2017.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationCapLED_2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHib-Mark-MDO47\GraduationCap2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,11 @@
     <sheet name="CapDesign" sheetId="2" r:id="rId1"/>
     <sheet name="AltCapDesign" sheetId="3" r:id="rId2"/>
     <sheet name="PictureRing" sheetId="1" r:id="rId3"/>
+    <sheet name="PowerDetails" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="battFactor">PowerDetails!$Q$57</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
   <si>
     <t>LED count</t>
   </si>
@@ -116,17 +120,490 @@
   </si>
   <si>
     <t>angle of diag</t>
+  </si>
+  <si>
+    <t>Chipset</t>
+  </si>
+  <si>
+    <t>Supported</t>
+  </si>
+  <si>
+    <t>Wires</t>
+  </si>
+  <si>
+    <t>Color Bits</t>
+  </si>
+  <si>
+    <t>Data Rate</t>
+  </si>
+  <si>
+    <t>PWM Rate</t>
+  </si>
+  <si>
+    <t>Chipset Power Draw</t>
+  </si>
+  <si>
+    <t>APA102/DOTSTAR</t>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
+    <t>~24Mbps</t>
+  </si>
+  <si>
+    <t>20khz</t>
+  </si>
+  <si>
+    <t>0.9ma@5v</t>
+  </si>
+  <si>
+    <t>WS2811</t>
+  </si>
+  <si>
+    <t>800kbps</t>
+  </si>
+  <si>
+    <t>400Hz</t>
+  </si>
+  <si>
+    <t>5mw / 1ma@5v</t>
+  </si>
+  <si>
+    <t>WS2812B/NEOPIXEL</t>
+  </si>
+  <si>
+    <t>TM1809/TM1812</t>
+  </si>
+  <si>
+    <t>7.2mw / 0.6ma@12v</t>
+  </si>
+  <si>
+    <t>TM1803</t>
+  </si>
+  <si>
+    <t>400kbps</t>
+  </si>
+  <si>
+    <t>TM1804</t>
+  </si>
+  <si>
+    <t>WS2801</t>
+  </si>
+  <si>
+    <t>1Mbps</t>
+  </si>
+  <si>
+    <t>2.5kHz</t>
+  </si>
+  <si>
+    <t>60mw / 5ma@12v</t>
+  </si>
+  <si>
+    <t>UCS1903</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>UCS2903</t>
+  </si>
+  <si>
+    <t>LPD8806</t>
+  </si>
+  <si>
+    <t>1-20Mbps</t>
+  </si>
+  <si>
+    <t>4kHz</t>
+  </si>
+  <si>
+    <t>P9813</t>
+  </si>
+  <si>
+    <t>1-15Mbps</t>
+  </si>
+  <si>
+    <t>4.5kHz</t>
+  </si>
+  <si>
+    <t>SM16716</t>
+  </si>
+  <si>
+    <t>TM1829</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>1.6Mbps/800kbps</t>
+  </si>
+  <si>
+    <t>7kHz</t>
+  </si>
+  <si>
+    <t>6ma@12v</t>
+  </si>
+  <si>
+    <t>TLS3001</t>
+  </si>
+  <si>
+    <t>TLC5940</t>
+  </si>
+  <si>
+    <t>TLC5947</t>
+  </si>
+  <si>
+    <t>LPD1886</t>
+  </si>
+  <si>
+    <t>Chipset power draw is how much power a single chip draws when the leds are off, but power is connected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  https://github.com/FastLED/FastLED/wiki/Chipset-reference</t>
+  </si>
+  <si>
+    <r>
+      <t>ws2811/ws2812/ws2812B - (adafruit sells these as "neopixels") super cheap (30 leds/m for $6, 60 leds/m for $11!), very slow data rate (800Kbps - meaning you'd want to investigate parallel output for more than a few hundred leds - see paul's excellent OctoWS2811 if you're using a teensy 3 - and i'm currently working on code for FastLED that will allow grouping/blocking of multiple streams of output in parallel - hopefully that will be out some time this year - I had an installation going in on july 4th that used it :). Also - many of the strips are 1 led, 1 controller, so you can cut at every led. Even better, is the ws2812 variant, which is the led and chip in a single package (some people still sell these as ws2811 - but the protocol is the same) - so it can be very very compact. Unfortunately, their data protocol requires disabling interrupts on the avr while writing data out, and so using these leds will interfere with things like IR libraries or using i2c and serial. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> at some point, the timings for WS2811 chips changed to be closer in line to the WS2812 timings. If you have chips identified as WS2811 that are behaving badly, try changing the chipset reference in addLEds to WS2812, and see if that fixes the issues.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://fastled.io/docs/3.1/group___power.html</t>
+  </si>
+  <si>
+    <r>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> uint8_t gRed_mW = 16 * 5; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 16mA @ 5v = 80mW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> uint8_t gGreen_mW = 11 * 5; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 11mA @ 5v = 55mW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> uint8_t gBlue_mW = 15 * 5; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 15mA @ 5v = 75mW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> uint8_t gDark_mW = 1 * 5; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 1mA @ 5v = 5mW</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://fastled.io/docs/3.1/power__mgt_8cpp_source.html</t>
+  </si>
+  <si>
+    <t>#define NUM_LEDS    93</t>
+  </si>
+  <si>
+    <t>#define BRIGHTNESS         255</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 1500); // WHITE</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 1500); // RED</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 1500); // GREEN</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 1500); // BLUE</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 500); // WHITE</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 500); // RED</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 500); // GREEN</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 500); // BLUE</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 3968); // WHITE</t>
+  </si>
+  <si>
+    <t>uint8_t pwrBright = calculate_max_brightness_for_power_vmA(leds, NUM_LEDS, BRIGHTNESS, 5, 3967); // WHITE</t>
+  </si>
+  <si>
+    <t>93 LEDs White</t>
+  </si>
+  <si>
+    <t>93 LEDs Red</t>
+  </si>
+  <si>
+    <t>93 LEDs Green</t>
+  </si>
+  <si>
+    <t>93 LEDs Blue</t>
+  </si>
+  <si>
+    <t>Battery Capacity</t>
+  </si>
+  <si>
+    <t>Battery Type</t>
+  </si>
+  <si>
+    <t>Capacity (mAh)</t>
+  </si>
+  <si>
+    <t>Typical Drain (mA)</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>9 Volt</t>
+  </si>
+  <si>
+    <t>Volts</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Power Drain</t>
+  </si>
+  <si>
+    <t>Time (h)</t>
+  </si>
+  <si>
+    <t>how many</t>
+  </si>
+  <si>
+    <t>my drain</t>
+  </si>
+  <si>
+    <t>my time</t>
+  </si>
+  <si>
+    <t>total battery</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>all white but one red expt - using 9V battery - battery drained quickly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   https://www.parts-express.com/shoppingcart.aspx 50 4-carriers for C-cell @ $1.02 = $51</t>
+  </si>
+  <si>
+    <t>banggood.com</t>
+  </si>
+  <si>
+    <t>ZTW 6A BEC UBEC Universal Battery Eliminator Circuit For RC Models (989402)</t>
+  </si>
+  <si>
+    <t>Soloop 328pcs 2:1 Polyolefin Halogen-Free Heat Shrink Tube Sleeving 5 Color 8 Size (969574)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,16 +627,89 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF003366"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -167,18 +717,242 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9900FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9900FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9900FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9900FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF330099"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9900FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF330099"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9900FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9900FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9900FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF330099"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9900FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9900FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF330099"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF330099"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9900FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF330099"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9900FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9900FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9900FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9900FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF330099"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9900FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9900FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF330099"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9900FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9900FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF330099"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9900FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9900FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9900FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF330099"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9900FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF330099"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9900FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF330099"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -923,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AB116" sqref="AB116"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AQ27" sqref="AQ27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,7 +1915,7 @@
         <v>69.913749999999993</v>
       </c>
       <c r="AA102" s="4">
-        <f t="shared" ref="AA101:AA102" si="0">SQRT(POWER(W102,2)+POWER(Y102,2))</f>
+        <f t="shared" ref="AA102" si="0">SQRT(POWER(W102,2)+POWER(Y102,2))</f>
         <v>110.0713187125738</v>
       </c>
     </row>
@@ -1278,4 +2052,961 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V76"/>
+  <sheetViews>
+    <sheetView topLeftCell="H57" workbookViewId="0">
+      <selection activeCell="S70" sqref="S70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="121.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7">
+        <v>8</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>8</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8">
+        <v>7</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>8</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="8">
+        <v>12</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7">
+        <v>12</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="8">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="7">
+        <v>3</v>
+      </c>
+      <c r="D20" s="7">
+        <v>12</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="189.75" x14ac:dyDescent="0.25">
+      <c r="I22" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>11</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>96</v>
+      </c>
+      <c r="I35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>243</v>
+      </c>
+      <c r="I36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>255</v>
+      </c>
+      <c r="I37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>255</v>
+      </c>
+      <c r="I38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>32</v>
+      </c>
+      <c r="I40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>81</v>
+      </c>
+      <c r="I41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>211</v>
+      </c>
+      <c r="I42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>86</v>
+      </c>
+      <c r="I43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>254</v>
+      </c>
+      <c r="I45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>255</v>
+      </c>
+      <c r="I46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <f>93*SUM(H28:H31)</f>
+        <v>3999</v>
+      </c>
+      <c r="I49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <f>93*(H28+H$31)</f>
+        <v>1581</v>
+      </c>
+      <c r="I50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <f>93*(H29+H$31)</f>
+        <v>1116</v>
+      </c>
+      <c r="I51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <f>93*(H30+H$31)</f>
+        <v>1488</v>
+      </c>
+      <c r="I52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>2100</v>
+      </c>
+      <c r="I54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q57">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="58" spans="8:22" x14ac:dyDescent="0.25">
+      <c r="K58" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="8:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K59" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="L59" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="M59" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="N59" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="8:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K60" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="L60" s="16">
+        <v>2400</v>
+      </c>
+      <c r="M60" s="16">
+        <v>50</v>
+      </c>
+      <c r="N60">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="61" spans="8:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K61" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L61" s="16">
+        <v>1000</v>
+      </c>
+      <c r="M61" s="16">
+        <v>10</v>
+      </c>
+      <c r="N61">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="62" spans="8:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K62" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="L62" s="16">
+        <v>500</v>
+      </c>
+      <c r="M62" s="16">
+        <v>15</v>
+      </c>
+      <c r="N62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="8:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="K64" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="L64" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="M64" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="O64" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="P64" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q64" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="R64" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="S64" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="T64" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="V64" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="11:22" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K65" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="L65" s="18">
+        <v>13000</v>
+      </c>
+      <c r="M65" s="23">
+        <v>200</v>
+      </c>
+      <c r="N65">
+        <v>1.5</v>
+      </c>
+      <c r="O65">
+        <f>L65*N65</f>
+        <v>19500</v>
+      </c>
+      <c r="P65">
+        <f>M65*N65</f>
+        <v>300</v>
+      </c>
+      <c r="Q65">
+        <f>ROUND(L65*battFactor/M65,0)</f>
+        <v>46</v>
+      </c>
+      <c r="R65">
+        <v>1500</v>
+      </c>
+      <c r="S65">
+        <v>6</v>
+      </c>
+      <c r="T65" s="28">
+        <f>S65*L65*battFactor/R65</f>
+        <v>36.4</v>
+      </c>
+      <c r="V65">
+        <f>4*S65</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="11:22" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K66" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="L66" s="18">
+        <v>6000</v>
+      </c>
+      <c r="M66" s="23">
+        <v>100</v>
+      </c>
+      <c r="N66">
+        <v>1.5</v>
+      </c>
+      <c r="O66">
+        <f t="shared" ref="O66:O69" si="0">L66*N66</f>
+        <v>9000</v>
+      </c>
+      <c r="P66">
+        <f t="shared" ref="P66:P69" si="1">M66*N66</f>
+        <v>150</v>
+      </c>
+      <c r="Q66">
+        <f>ROUND(L66*battFactor/M66,0)</f>
+        <v>42</v>
+      </c>
+      <c r="R66">
+        <v>1500</v>
+      </c>
+      <c r="S66">
+        <v>6</v>
+      </c>
+      <c r="T66" s="28">
+        <f>S66*L66*battFactor/R66</f>
+        <v>16.8</v>
+      </c>
+      <c r="V66">
+        <f t="shared" ref="V66:V69" si="2">4*S66</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="11:22" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K67" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="L67" s="18">
+        <v>2400</v>
+      </c>
+      <c r="M67" s="23">
+        <v>50</v>
+      </c>
+      <c r="N67">
+        <v>1.5</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="Q67">
+        <f>ROUND(L67*battFactor/M67,0)</f>
+        <v>34</v>
+      </c>
+      <c r="R67">
+        <v>1500</v>
+      </c>
+      <c r="S67">
+        <v>6</v>
+      </c>
+      <c r="T67" s="28">
+        <f>S67*L67*battFactor/R67</f>
+        <v>6.72</v>
+      </c>
+      <c r="V67">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="11:22" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K68" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L68" s="18">
+        <v>1000</v>
+      </c>
+      <c r="M68" s="23">
+        <v>10</v>
+      </c>
+      <c r="N68">
+        <v>1.5</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Q68">
+        <f>ROUND(L68*battFactor/M68,0)</f>
+        <v>70</v>
+      </c>
+      <c r="R68">
+        <v>1500</v>
+      </c>
+      <c r="S68">
+        <v>6</v>
+      </c>
+      <c r="T68" s="28">
+        <f>S68*L68*battFactor/R68</f>
+        <v>2.8</v>
+      </c>
+      <c r="V68">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="11:22" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K69" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="L69" s="25">
+        <v>500</v>
+      </c>
+      <c r="M69" s="26">
+        <v>15</v>
+      </c>
+      <c r="N69">
+        <v>9</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="Q69">
+        <f>ROUND(L69*battFactor/M69,0)</f>
+        <v>23</v>
+      </c>
+      <c r="R69">
+        <v>1500</v>
+      </c>
+      <c r="S69">
+        <v>1</v>
+      </c>
+      <c r="T69" s="29">
+        <f>S69*L69*battFactor/R69</f>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="V69">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K72" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K74" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="L75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="L76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some new letters for POLY 2018
</commit_message>
<xml_diff>
--- a/GraduationCapDesign_2017.xlsx
+++ b/GraduationCapDesign_2017.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="179">
   <si>
     <t>LED count</t>
   </si>
@@ -704,12 +704,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66, 46, -1 };</t>
-  </si>
-  <si>
-    <t>const char ltr_T[14] = { -13, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78, 64, 44 };</t>
-  </si>
-  <si>
     <t>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90, 92, 86 };</t>
   </si>
   <si>
@@ -729,6 +723,84 @@
   </si>
   <si>
     <t>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92 };</t>
+  </si>
+  <si>
+    <t>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78, 64, 44 };</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Power Banks RAVPower 22000 Portable Charger 22000mAh 5.8A Output 3-Port Battery Pack (2.4A Input, iSmart 2.0 USB Ports, Li-polymer Battery Banks) Portable Battery Charger For Smartphone Tablet – Black</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/RAVPower-Portable-22000mAh-Li-polymer-Smartphone/dp/B01G1XH46M/ref=sr_1_1_sspa?ie=UTF8&amp;qid=1515301821&amp;sr=8-1-spons&amp;keywords=battery+power+pack&amp;psc=1</t>
+  </si>
+  <si>
+    <t>$39.99  | FREE One-Day  - currently a 10% off coupon</t>
+  </si>
+  <si>
+    <t>per hour</t>
+  </si>
+  <si>
+    <t>Portable Charger RAVPower 26800 Battery Packs 26800mAh Total 5.5A Output 3-Port…</t>
+  </si>
+  <si>
+    <t>$49.99  | FREE One-Day - currently 5% off</t>
+  </si>
+  <si>
+    <t>Power Banks 32000 RAVPower 32000mAh 6A Output Portable Charger, External Battery Pack (3…</t>
+  </si>
+  <si>
+    <r>
+      <t>$59.99</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF111111"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>  | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF111111"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>FREE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF111111"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> One-Day</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$33.99  | FREE One-Day </t>
+  </si>
+  <si>
+    <t>[Upgraded] Poweradd Pilot Pro3 30000mAh Power Bank (Dual Inputs/4A, 3 Outputs…</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66, 46 };</t>
+  </si>
+  <si>
+    <t>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64, 63, 41 };</t>
+  </si>
+  <si>
+    <t>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74, 58, 35 };</t>
   </si>
 </sst>
 </file>
@@ -740,7 +812,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,6 +922,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1059,7 +1144,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1142,6 +1227,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2490,22 +2578,22 @@
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
-      <c r="T2" s="38" t="s">
+      <c r="T2" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
       <c r="X2" s="35"/>
       <c r="Y2" t="s">
         <v>147</v>
       </c>
-      <c r="Z2" s="38" t="s">
+      <c r="Z2" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
     </row>
     <row r="3" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G3" s="33" t="s">
@@ -9014,2015 +9102,2203 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W96"/>
+  <dimension ref="A2:AA96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="9" width="3.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="1" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="11" width="3.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="15" max="17" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="E2" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="F2" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35">
         <v>2</v>
       </c>
-      <c r="G2" s="35">
-        <v>0</v>
-      </c>
-      <c r="H2" s="35">
-        <v>1</v>
-      </c>
       <c r="I2" s="35">
+        <v>0</v>
+      </c>
+      <c r="J2" s="35">
+        <v>1</v>
+      </c>
+      <c r="K2" s="35">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>155</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="O2" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="P2" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q2" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="R2" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="S2" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="T2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36">
+      <c r="U2" s="36"/>
+      <c r="V2" s="36">
         <v>2</v>
       </c>
-      <c r="S2" s="36">
-        <v>0</v>
-      </c>
-      <c r="T2" s="36">
-        <v>1</v>
-      </c>
-      <c r="U2" s="36">
+      <c r="W2" s="36">
+        <v>0</v>
+      </c>
+      <c r="X2" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="36">
         <v>8</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>-COUNTA(A4:A96)</f>
         <v>-17</v>
       </c>
       <c r="B3">
-        <f>-COUNTA(B4:B96)</f>
+        <f t="shared" ref="B3:C3" si="0">-COUNTA(B4:B96)</f>
+        <v>-10</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
         <v>-12</v>
-      </c>
-      <c r="C3">
-        <f>-COUNTA(C4:C96)</f>
-        <v>-17</v>
       </c>
       <c r="D3">
         <f>-COUNTA(D4:D96)</f>
+        <v>-12</v>
+      </c>
+      <c r="E3">
+        <f>-COUNTA(E4:E96)</f>
         <v>-17</v>
       </c>
       <c r="F3">
         <f>-COUNTA(F4:F96)</f>
         <v>-17</v>
       </c>
-      <c r="G3">
-        <f>-COUNTA(G4:G96)</f>
-        <v>-24</v>
-      </c>
       <c r="H3">
         <f>-COUNTA(H4:H96)</f>
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="I3">
         <f>-COUNTA(I4:I96)</f>
         <v>-24</v>
       </c>
+      <c r="J3">
+        <f>-COUNTA(J4:J96)</f>
+        <v>-15</v>
+      </c>
       <c r="K3">
         <f>-COUNTA(K4:K96)</f>
+        <v>-24</v>
+      </c>
+      <c r="M3">
+        <f>-COUNTA(M4:M96)</f>
         <v>-93</v>
       </c>
-      <c r="M3" t="str">
-        <f>"const char ltr_"&amp;M2&amp;"["&amp;1-A3&amp;"] = { "&amp;A3</f>
+      <c r="O3" t="str">
+        <f>"const char ltr_"&amp;O2&amp;"["&amp;1-A3&amp;"] = { "&amp;A3</f>
         <v>const char ltr_P[18] = { -17</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:P3" si="0">"const char ltr_"&amp;N2&amp;"["&amp;1-B3&amp;"] = { "&amp;B3</f>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:Q3" si="1">"const char ltr_"&amp;P2&amp;"["&amp;1-B3&amp;"] = { "&amp;B3</f>
+        <v>const char ltr_L[11] = { -10</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" si="1"/>
+        <v>const char ltr_Y[13] = { -12</v>
+      </c>
+      <c r="R3" t="str">
+        <f>"const char ltr_"&amp;R2&amp;"["&amp;1-D3&amp;"] = { "&amp;D3</f>
         <v>const char ltr_T[13] = { -12</v>
       </c>
-      <c r="O3" t="str">
-        <f t="shared" si="0"/>
+      <c r="S3" t="str">
+        <f>"const char ltr_"&amp;S2&amp;"["&amp;1-E3&amp;"] = { "&amp;E3</f>
         <v>const char ltr_H[18] = { -17</v>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" si="0"/>
+      <c r="T3" t="str">
+        <f>"const char ltr_"&amp;T2&amp;"["&amp;1-F3&amp;"] = { "&amp;F3</f>
         <v>const char ltr_S[18] = { -17</v>
       </c>
-      <c r="R3" t="str">
-        <f t="shared" ref="R3:U3" si="1">"const char ltr_"&amp;R2&amp;"["&amp;1-F3&amp;"] = { "&amp;F3</f>
+      <c r="V3" t="str">
+        <f>"const char ltr_"&amp;V2&amp;"["&amp;1-H3&amp;"] = { "&amp;H3</f>
         <v>const char ltr_2[18] = { -17</v>
       </c>
-      <c r="S3" t="str">
-        <f t="shared" si="1"/>
+      <c r="W3" t="str">
+        <f>"const char ltr_"&amp;W2&amp;"["&amp;1-I3&amp;"] = { "&amp;I3</f>
         <v>const char ltr_0[25] = { -24</v>
       </c>
-      <c r="T3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X3" t="str">
+        <f>"const char ltr_"&amp;X2&amp;"["&amp;1-J3&amp;"] = { "&amp;J3</f>
         <v>const char ltr_1[16] = { -15</v>
       </c>
-      <c r="U3" t="str">
-        <f t="shared" si="1"/>
+      <c r="Y3" t="str">
+        <f>"const char ltr_"&amp;Y2&amp;"["&amp;1-K3&amp;"] = { "&amp;K3</f>
         <v>const char ltr_8[25] = { -24</v>
       </c>
-      <c r="W3" t="str">
-        <f>"const char ltr_"&amp;W2&amp;"["&amp;1-K3&amp;"] = { "&amp;K3</f>
+      <c r="AA3" t="str">
+        <f>"const char ltr_"&amp;AA2&amp;"["&amp;1-M3&amp;"] = { "&amp;M3</f>
         <v>const char ltr_all[94] = { -93</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>81</v>
       </c>
       <c r="B4">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <v>78</v>
+      </c>
+      <c r="D4">
         <v>53</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>54</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>34</v>
-      </c>
-      <c r="F4">
-        <v>53</v>
-      </c>
-      <c r="G4">
-        <v>32</v>
       </c>
       <c r="H4">
         <v>53</v>
       </c>
       <c r="I4">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>53</v>
+      </c>
+      <c r="K4">
         <v>54</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="str">
-        <f>M3&amp;", "&amp;A4</f>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="str">
+        <f>O3&amp;", "&amp;A4</f>
         <v>const char ltr_P[18] = { -17, 81</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" ref="N4:N20" si="2">N3&amp;", "&amp;B4</f>
+      <c r="P4" t="str">
+        <f t="shared" ref="P4:Q15" si="2">P3&amp;", "&amp;B4</f>
+        <v>const char ltr_L[11] = { -10, 54</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" ref="R4:R15" si="3">R3&amp;", "&amp;D4</f>
         <v>const char ltr_T[13] = { -12, 53</v>
       </c>
-      <c r="O4" t="str">
-        <f t="shared" ref="O4:O20" si="3">O3&amp;", "&amp;C4</f>
+      <c r="S4" t="str">
+        <f t="shared" ref="S4:S20" si="4">S3&amp;", "&amp;E4</f>
         <v>const char ltr_H[18] = { -17, 54</v>
       </c>
-      <c r="P4" t="str">
-        <f t="shared" ref="P4:P20" si="4">P3&amp;", "&amp;D4</f>
+      <c r="T4" t="str">
+        <f t="shared" ref="T4:T20" si="5">T3&amp;", "&amp;F4</f>
         <v>const char ltr_S[18] = { -17, 34</v>
       </c>
-      <c r="R4" t="str">
-        <f t="shared" ref="R4:R20" si="5">R3&amp;", "&amp;F4</f>
+      <c r="V4" t="str">
+        <f t="shared" ref="V4:V20" si="6">V3&amp;", "&amp;H4</f>
         <v>const char ltr_2[18] = { -17, 53</v>
       </c>
-      <c r="S4" t="str">
-        <f t="shared" ref="S4:S27" si="6">S3&amp;", "&amp;G4</f>
+      <c r="W4" t="str">
+        <f t="shared" ref="W4:W27" si="7">W3&amp;", "&amp;I4</f>
         <v>const char ltr_0[25] = { -24, 32</v>
       </c>
-      <c r="T4" t="str">
-        <f t="shared" ref="T4:T18" si="7">T3&amp;", "&amp;H4</f>
+      <c r="X4" t="str">
+        <f t="shared" ref="X4:X18" si="8">X3&amp;", "&amp;J4</f>
         <v>const char ltr_1[16] = { -15, 53</v>
       </c>
-      <c r="U4" t="str">
-        <f t="shared" ref="U4:W27" si="8">U3&amp;", "&amp;I4</f>
+      <c r="Y4" t="str">
+        <f>Y3&amp;", "&amp;K4</f>
         <v>const char ltr_8[25] = { -24, 54</v>
       </c>
-      <c r="W4" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA4" t="str">
+        <f>AA3&amp;", "&amp;M4</f>
         <v>const char ltr_all[94] = { -93, 0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>82</v>
       </c>
       <c r="B5">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5">
         <v>71</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>70</v>
       </c>
-      <c r="D5">
-        <v>33</v>
-      </c>
       <c r="F5">
-        <v>54</v>
-      </c>
-      <c r="G5">
         <v>33</v>
       </c>
       <c r="H5">
         <v>54</v>
       </c>
       <c r="I5">
+        <v>33</v>
+      </c>
+      <c r="J5">
+        <v>54</v>
+      </c>
+      <c r="K5">
         <v>55</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" ref="M5:M19" si="9">M4&amp;", "&amp;A5</f>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" ref="O5:O11" si="9">O4&amp;", "&amp;A5</f>
         <v>const char ltr_P[18] = { -17, 81, 82</v>
       </c>
-      <c r="N5" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64</v>
+      </c>
+      <c r="R5" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71</v>
       </c>
-      <c r="O5" t="str">
-        <f t="shared" si="3"/>
+      <c r="S5" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70</v>
       </c>
-      <c r="P5" t="str">
-        <f t="shared" si="4"/>
+      <c r="T5" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33</v>
       </c>
-      <c r="R5" t="str">
-        <f t="shared" si="5"/>
+      <c r="V5" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54</v>
       </c>
-      <c r="S5" t="str">
-        <f t="shared" si="6"/>
+      <c r="W5" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33</v>
       </c>
-      <c r="T5" t="str">
-        <f t="shared" si="7"/>
+      <c r="X5" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54</v>
       </c>
-      <c r="U5" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y5" t="str">
+        <f>Y4&amp;", "&amp;K5</f>
         <v>const char ltr_8[25] = { -24, 54, 55</v>
       </c>
-      <c r="W5" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA5" t="str">
+        <f>AA4&amp;", "&amp;M5</f>
         <v>const char ltr_all[94] = { -93, 0, 1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>70</v>
       </c>
       <c r="B6">
+        <v>82</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+      <c r="D6">
         <v>56</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>82</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>32</v>
-      </c>
-      <c r="F6">
-        <v>55</v>
-      </c>
-      <c r="G6">
-        <v>34</v>
       </c>
       <c r="H6">
         <v>55</v>
       </c>
       <c r="I6">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>55</v>
+      </c>
+      <c r="K6">
         <v>32</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>2</v>
       </c>
-      <c r="M6" t="str">
+      <c r="O6" t="str">
         <f t="shared" si="9"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70</v>
       </c>
-      <c r="N6" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56</v>
       </c>
-      <c r="O6" t="str">
-        <f t="shared" si="3"/>
+      <c r="S6" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82</v>
       </c>
-      <c r="P6" t="str">
-        <f t="shared" si="4"/>
+      <c r="T6" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32</v>
       </c>
-      <c r="R6" t="str">
-        <f t="shared" si="5"/>
+      <c r="V6" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55</v>
       </c>
-      <c r="S6" t="str">
-        <f t="shared" si="6"/>
+      <c r="W6" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34</v>
       </c>
-      <c r="T6" t="str">
-        <f t="shared" si="7"/>
+      <c r="X6" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55</v>
       </c>
-      <c r="U6" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y6" t="str">
+        <f>Y5&amp;", "&amp;K6</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32</v>
       </c>
-      <c r="W6" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA6" t="str">
+        <f>AA5&amp;", "&amp;M6</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>54</v>
       </c>
       <c r="B7">
+        <v>81</v>
+      </c>
+      <c r="C7">
+        <v>53</v>
+      </c>
+      <c r="D7">
         <v>57</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>81</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>55</v>
-      </c>
-      <c r="F7">
-        <v>32</v>
-      </c>
-      <c r="G7">
-        <v>35</v>
       </c>
       <c r="H7">
         <v>32</v>
       </c>
       <c r="I7">
+        <v>35</v>
+      </c>
+      <c r="J7">
+        <v>32</v>
+      </c>
+      <c r="K7">
         <v>33</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>3</v>
       </c>
-      <c r="M7" t="str">
+      <c r="O7" t="str">
         <f t="shared" si="9"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54</v>
       </c>
-      <c r="N7" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57</v>
       </c>
-      <c r="O7" t="str">
-        <f t="shared" si="3"/>
+      <c r="S7" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81</v>
       </c>
-      <c r="P7" t="str">
-        <f t="shared" si="4"/>
+      <c r="T7" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55</v>
       </c>
-      <c r="R7" t="str">
-        <f t="shared" si="5"/>
+      <c r="V7" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32</v>
       </c>
-      <c r="S7" t="str">
-        <f t="shared" si="6"/>
+      <c r="W7" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35</v>
       </c>
-      <c r="T7" t="str">
-        <f t="shared" si="7"/>
+      <c r="X7" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32</v>
       </c>
-      <c r="U7" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y7" t="str">
+        <f>Y6&amp;", "&amp;K7</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33</v>
       </c>
-      <c r="W7" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA7" t="str">
+        <f>AA6&amp;", "&amp;M7</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>55</v>
       </c>
       <c r="B8">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>70</v>
+      </c>
+      <c r="D8">
         <v>35</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>80</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>54</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>33</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>36</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>56</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>34</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>4</v>
       </c>
-      <c r="M8" t="str">
+      <c r="O8" t="str">
         <f t="shared" si="9"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55</v>
       </c>
-      <c r="N8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35</v>
       </c>
-      <c r="O8" t="str">
-        <f t="shared" si="3"/>
+      <c r="S8" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80</v>
       </c>
-      <c r="P8" t="str">
-        <f t="shared" si="4"/>
+      <c r="T8" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54</v>
       </c>
-      <c r="R8" t="str">
-        <f t="shared" si="5"/>
+      <c r="V8" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33</v>
       </c>
-      <c r="S8" t="str">
-        <f t="shared" si="6"/>
+      <c r="W8" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36</v>
       </c>
-      <c r="T8" t="str">
-        <f t="shared" si="7"/>
+      <c r="X8" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56</v>
       </c>
-      <c r="U8" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y8" t="str">
+        <f>Y7&amp;", "&amp;K8</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34</v>
       </c>
-      <c r="W8" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA8" t="str">
+        <f>AA7&amp;", "&amp;M8</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32</v>
       </c>
       <c r="B9">
+        <v>66</v>
+      </c>
+      <c r="C9">
+        <v>82</v>
+      </c>
+      <c r="D9">
         <v>72</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>66</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>70</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>34</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>37</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>72</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>58</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>5</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <f t="shared" si="9"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" si="3"/>
+      <c r="S9" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66</v>
       </c>
-      <c r="P9" t="str">
-        <f t="shared" si="4"/>
+      <c r="T9" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70</v>
       </c>
-      <c r="R9" t="str">
-        <f t="shared" si="5"/>
+      <c r="V9" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34</v>
       </c>
-      <c r="S9" t="str">
-        <f t="shared" si="6"/>
+      <c r="W9" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37</v>
       </c>
-      <c r="T9" t="str">
-        <f t="shared" si="7"/>
+      <c r="X9" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72</v>
       </c>
-      <c r="U9" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y9" t="str">
+        <f>Y8&amp;", "&amp;K9</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58</v>
       </c>
-      <c r="W9" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA9" t="str">
+        <f>AA8&amp;", "&amp;M9</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>33</v>
       </c>
       <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+      <c r="D10">
         <v>84</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>46</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>82</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>35</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>38</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>84</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>74</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>6</v>
       </c>
-      <c r="M10" t="str">
+      <c r="O10" t="str">
         <f t="shared" si="9"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33</v>
       </c>
-      <c r="N10" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84</v>
       </c>
-      <c r="O10" t="str">
-        <f t="shared" si="3"/>
+      <c r="S10" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46</v>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" si="4"/>
+      <c r="T10" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82</v>
       </c>
-      <c r="R10" t="str">
-        <f t="shared" si="5"/>
+      <c r="V10" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35</v>
       </c>
-      <c r="S10" t="str">
-        <f t="shared" si="6"/>
+      <c r="W10" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38</v>
       </c>
-      <c r="T10" t="str">
-        <f t="shared" si="7"/>
+      <c r="X10" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84</v>
       </c>
-      <c r="U10" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y10" t="str">
+        <f>Y9&amp;", "&amp;K10</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74</v>
       </c>
-      <c r="W10" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA10" t="str">
+        <f>AA9&amp;", "&amp;M10</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
       <c r="B11">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
         <v>92</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>34</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>91</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>58</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>39</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>92</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>85</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>7</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <f t="shared" si="9"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34</v>
       </c>
-      <c r="N11" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92</v>
       </c>
-      <c r="O11" t="str">
-        <f t="shared" si="3"/>
+      <c r="S11" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34</v>
       </c>
-      <c r="P11" t="str">
-        <f t="shared" si="4"/>
+      <c r="T11" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91</v>
       </c>
-      <c r="R11" t="str">
-        <f t="shared" si="5"/>
+      <c r="V11" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58</v>
       </c>
-      <c r="S11" t="str">
-        <f t="shared" si="6"/>
+      <c r="W11" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39</v>
       </c>
-      <c r="T11" t="str">
-        <f t="shared" si="7"/>
+      <c r="X11" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92</v>
       </c>
-      <c r="U11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y11" t="str">
+        <f>Y10&amp;", "&amp;K11</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85</v>
       </c>
-      <c r="W11" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA11" t="str">
+        <f>AA10&amp;", "&amp;M11</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
       <c r="B12">
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <v>86</v>
+      </c>
+      <c r="D12">
         <v>88</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>58</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>92</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>85</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>40</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>88</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>92</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>8</v>
       </c>
-      <c r="M12" t="str">
-        <f>M11&amp;", "&amp;A13</f>
+      <c r="O12" t="str">
+        <f t="shared" ref="O12:O20" si="10">O11&amp;", "&amp;A13</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59</v>
       </c>
-      <c r="N12" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64, 63</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88</v>
       </c>
-      <c r="O12" t="str">
-        <f t="shared" si="3"/>
+      <c r="S12" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58</v>
       </c>
-      <c r="P12" t="str">
-        <f t="shared" si="4"/>
+      <c r="T12" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92</v>
       </c>
-      <c r="R12" t="str">
-        <f t="shared" si="5"/>
+      <c r="V12" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85</v>
       </c>
-      <c r="S12" t="str">
-        <f t="shared" si="6"/>
+      <c r="W12" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40</v>
       </c>
-      <c r="T12" t="str">
-        <f t="shared" si="7"/>
+      <c r="X12" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88</v>
       </c>
-      <c r="U12" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y12" t="str">
+        <f>Y11&amp;", "&amp;K12</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92</v>
       </c>
-      <c r="W12" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA12" t="str">
+        <f>AA11&amp;", "&amp;M12</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59</v>
       </c>
       <c r="B13">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>74</v>
       </c>
       <c r="D13">
+        <v>78</v>
+      </c>
+      <c r="E13">
+        <v>74</v>
+      </c>
+      <c r="F13">
         <v>87</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>92</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>41</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>78</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>89</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>9</v>
       </c>
-      <c r="M13" t="str">
-        <f>M12&amp;", "&amp;A14</f>
+      <c r="O13" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75</v>
       </c>
-      <c r="N13" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64, 63, 41</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74</v>
+      </c>
+      <c r="R13" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78</v>
       </c>
-      <c r="O13" t="str">
-        <f t="shared" si="3"/>
+      <c r="S13" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74</v>
       </c>
-      <c r="P13" t="str">
-        <f t="shared" si="4"/>
+      <c r="T13" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87</v>
       </c>
-      <c r="R13" t="str">
-        <f t="shared" si="5"/>
+      <c r="V13" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92</v>
       </c>
-      <c r="S13" t="str">
-        <f t="shared" si="6"/>
+      <c r="W13" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41</v>
       </c>
-      <c r="T13" t="str">
-        <f t="shared" si="7"/>
+      <c r="X13" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78</v>
       </c>
-      <c r="U13" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y13" t="str">
+        <f>Y12&amp;", "&amp;K13</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89</v>
       </c>
-      <c r="W13" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA13" t="str">
+        <f>AA12&amp;", "&amp;M13</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>75</v>
       </c>
-      <c r="B14">
+      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="D14">
         <v>64</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>75</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>76</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>89</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>42</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>47</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>80</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>10</v>
       </c>
-      <c r="M14" t="str">
-        <f>M13&amp;", "&amp;A15</f>
+      <c r="O14" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86</v>
       </c>
-      <c r="N14" t="str">
+      <c r="Q14" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74, 58</v>
+      </c>
+      <c r="R14" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78, 64</v>
       </c>
-      <c r="O14" t="str">
-        <f t="shared" si="3"/>
+      <c r="S14" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75</v>
       </c>
-      <c r="P14" t="str">
-        <f t="shared" si="4"/>
+      <c r="T14" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76</v>
       </c>
-      <c r="R14" t="str">
-        <f t="shared" si="5"/>
+      <c r="V14" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89</v>
       </c>
-      <c r="S14" t="str">
-        <f t="shared" si="6"/>
+      <c r="W14" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42</v>
       </c>
-      <c r="T14" t="str">
-        <f t="shared" si="7"/>
+      <c r="X14" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47</v>
       </c>
-      <c r="U14" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y14" t="str">
+        <f>Y13&amp;", "&amp;K14</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80</v>
       </c>
-      <c r="W14" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA14" t="str">
+        <f>AA13&amp;", "&amp;M14</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>86</v>
       </c>
-      <c r="B15">
+      <c r="C15">
+        <v>35</v>
+      </c>
+      <c r="D15">
         <v>44</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>76</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>62</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>66</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>43</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>65</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>66</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>11</v>
       </c>
-      <c r="M15" t="str">
-        <f>M14&amp;", "&amp;A16</f>
+      <c r="O15" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92</v>
       </c>
-      <c r="N15" t="str">
+      <c r="Q15" t="str">
         <f t="shared" si="2"/>
+        <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74, 58, 35</v>
+      </c>
+      <c r="R15" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78, 64, 44</v>
       </c>
-      <c r="O15" t="str">
-        <f t="shared" si="3"/>
+      <c r="S15" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76</v>
       </c>
-      <c r="P15" t="str">
-        <f t="shared" si="4"/>
+      <c r="T15" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62</v>
       </c>
-      <c r="R15" t="str">
-        <f t="shared" si="5"/>
+      <c r="V15" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66</v>
       </c>
-      <c r="S15" t="str">
-        <f t="shared" si="6"/>
+      <c r="W15" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43</v>
       </c>
-      <c r="T15" t="str">
-        <f t="shared" si="7"/>
+      <c r="X15" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65</v>
       </c>
-      <c r="U15" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y15" t="str">
+        <f>Y14&amp;", "&amp;K15</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66</v>
       </c>
-      <c r="W15" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA15" t="str">
+        <f>AA14&amp;", "&amp;M15</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>92</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>62</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>42</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>47</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>44</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>64</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>46</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>12</v>
       </c>
-      <c r="M16" t="str">
-        <f>M15&amp;", "&amp;A17</f>
+      <c r="O16" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90</v>
       </c>
-      <c r="O16" t="str">
-        <f t="shared" si="3"/>
+      <c r="S16" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62</v>
       </c>
-      <c r="P16" t="str">
-        <f t="shared" si="4"/>
+      <c r="T16" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42</v>
       </c>
-      <c r="R16" t="str">
-        <f t="shared" si="5"/>
+      <c r="V16" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47</v>
       </c>
-      <c r="S16" t="str">
-        <f t="shared" si="6"/>
+      <c r="W16" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44</v>
       </c>
-      <c r="T16" t="str">
-        <f t="shared" si="7"/>
+      <c r="X16" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64</v>
       </c>
-      <c r="U16" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y16" t="str">
+        <f>Y15&amp;", "&amp;K16</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46</v>
       </c>
-      <c r="W16" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA16" t="str">
+        <f>AA15&amp;", "&amp;M16</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>90</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>42</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>43</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>65</v>
-      </c>
-      <c r="G17">
-        <v>45</v>
-      </c>
-      <c r="H17">
-        <v>63</v>
       </c>
       <c r="I17">
         <v>45</v>
       </c>
+      <c r="J17">
+        <v>63</v>
+      </c>
       <c r="K17">
+        <v>45</v>
+      </c>
+      <c r="M17">
         <v>13</v>
       </c>
-      <c r="M17" t="str">
-        <f>M16&amp;", "&amp;A18</f>
+      <c r="O17" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80</v>
       </c>
-      <c r="O17" t="str">
-        <f t="shared" si="3"/>
+      <c r="S17" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42</v>
       </c>
-      <c r="P17" t="str">
-        <f t="shared" si="4"/>
+      <c r="T17" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43</v>
       </c>
-      <c r="R17" t="str">
-        <f t="shared" si="5"/>
+      <c r="V17" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65</v>
       </c>
-      <c r="S17" t="str">
-        <f t="shared" si="6"/>
+      <c r="W17" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45</v>
       </c>
-      <c r="T17" t="str">
-        <f t="shared" si="7"/>
+      <c r="X17" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64, 63</v>
       </c>
-      <c r="U17" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y17" t="str">
+        <f>Y16&amp;", "&amp;K17</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45</v>
       </c>
-      <c r="W17" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA17" t="str">
+        <f>AA16&amp;", "&amp;M17</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>90</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>44</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>64</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>46</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>41</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>44</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>14</v>
       </c>
-      <c r="M18" t="str">
-        <f>M17&amp;", "&amp;A19</f>
+      <c r="O18" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66</v>
       </c>
-      <c r="O18" t="str">
-        <f t="shared" si="3"/>
+      <c r="S18" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90</v>
       </c>
-      <c r="P18" t="str">
-        <f t="shared" si="4"/>
+      <c r="T18" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43, 44</v>
       </c>
-      <c r="R18" t="str">
-        <f t="shared" si="5"/>
+      <c r="V18" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65, 64</v>
       </c>
-      <c r="S18" t="str">
-        <f t="shared" si="6"/>
+      <c r="W18" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46</v>
       </c>
-      <c r="T18" t="str">
-        <f t="shared" si="7"/>
+      <c r="X18" t="str">
+        <f t="shared" si="8"/>
         <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64, 63, 41</v>
       </c>
-      <c r="U18" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y18" t="str">
+        <f>Y17&amp;", "&amp;K18</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44</v>
       </c>
-      <c r="W18" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA18" t="str">
+        <f>AA17&amp;", "&amp;M18</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>66</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>92</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>45</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>63</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>47</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>43</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>15</v>
       </c>
-      <c r="M19" t="str">
-        <f>M18&amp;", "&amp;A20</f>
+      <c r="O19" t="str">
+        <f t="shared" si="10"/>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66, 46</v>
       </c>
-      <c r="O19" t="str">
-        <f t="shared" si="3"/>
+      <c r="S19" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90, 92</v>
       </c>
-      <c r="P19" t="str">
-        <f t="shared" si="4"/>
+      <c r="T19" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43, 44, 45</v>
       </c>
-      <c r="R19" t="str">
-        <f t="shared" si="5"/>
+      <c r="V19" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65, 64, 63</v>
       </c>
-      <c r="S19" t="str">
-        <f t="shared" si="6"/>
+      <c r="W19" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47</v>
       </c>
-      <c r="U19" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y19" t="str">
+        <f>Y18&amp;", "&amp;K19</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43</v>
       </c>
-      <c r="W19" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA19" t="str">
+        <f>AA18&amp;", "&amp;M19</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>46</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>86</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>46</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>41</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>48</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>42</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>16</v>
       </c>
-      <c r="M20" t="str">
-        <f>M19&amp;", "&amp;A21</f>
+      <c r="O20" t="str">
+        <f t="shared" si="10"/>
         <v xml:space="preserve">const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66, 46, </v>
       </c>
-      <c r="O20" t="str">
-        <f t="shared" si="3"/>
+      <c r="S20" t="str">
+        <f t="shared" si="4"/>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90, 92, 86</v>
       </c>
-      <c r="P20" t="str">
-        <f t="shared" si="4"/>
+      <c r="T20" t="str">
+        <f t="shared" si="5"/>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43, 44, 45, 46</v>
       </c>
-      <c r="R20" t="str">
-        <f t="shared" si="5"/>
+      <c r="V20" t="str">
+        <f t="shared" si="6"/>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65, 64, 63, 41</v>
       </c>
-      <c r="S20" t="str">
-        <f t="shared" si="6"/>
+      <c r="W20" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48</v>
       </c>
-      <c r="U20" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y20" t="str">
+        <f>Y19&amp;", "&amp;K20</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42</v>
       </c>
-      <c r="W20" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA20" t="str">
+        <f>AA19&amp;", "&amp;M20</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G21">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I21">
         <v>49</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>62</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>17</v>
       </c>
-      <c r="S21" t="str">
-        <f t="shared" si="6"/>
+      <c r="W21" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49</v>
       </c>
-      <c r="U21" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y21" t="str">
+        <f>Y20&amp;", "&amp;K21</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62</v>
       </c>
-      <c r="W21" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA21" t="str">
+        <f>AA20&amp;", "&amp;M21</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G22">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I22">
         <v>50</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>76</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>18</v>
       </c>
-      <c r="S22" t="str">
-        <f t="shared" si="6"/>
+      <c r="W22" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50</v>
       </c>
-      <c r="U22" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y22" t="str">
+        <f>Y21&amp;", "&amp;K22</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76</v>
       </c>
-      <c r="W22" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA22" t="str">
+        <f>AA21&amp;", "&amp;M22</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G23">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I23">
         <v>51</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>87</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>19</v>
       </c>
-      <c r="S23" t="str">
-        <f t="shared" si="6"/>
+      <c r="W23" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51</v>
       </c>
-      <c r="U23" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y23" t="str">
+        <f>Y22&amp;", "&amp;K23</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87</v>
       </c>
-      <c r="W23" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA23" t="str">
+        <f>AA22&amp;", "&amp;M23</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G24">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I24">
         <v>52</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>91</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>20</v>
       </c>
-      <c r="S24" t="str">
-        <f t="shared" si="6"/>
+      <c r="W24" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52</v>
       </c>
-      <c r="U24" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y24" t="str">
+        <f>Y23&amp;", "&amp;K24</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91</v>
       </c>
-      <c r="W24" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA24" t="str">
+        <f>AA23&amp;", "&amp;M24</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I25">
         <v>53</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>82</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>21</v>
       </c>
-      <c r="S25" t="str">
-        <f t="shared" si="6"/>
+      <c r="W25" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53</v>
       </c>
-      <c r="U25" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y25" t="str">
+        <f>Y24&amp;", "&amp;K25</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91, 82</v>
       </c>
-      <c r="W25" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA25" t="str">
+        <f>AA24&amp;", "&amp;M25</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G26">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I26">
         <v>54</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>70</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>22</v>
       </c>
-      <c r="S26" t="str">
-        <f t="shared" si="6"/>
+      <c r="W26" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54</v>
       </c>
-      <c r="U26" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y26" t="str">
+        <f>Y25&amp;", "&amp;K26</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91, 82, 70</v>
       </c>
-      <c r="W26" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA26" t="str">
+        <f>AA25&amp;", "&amp;M26</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I27">
         <v>55</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>54</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>23</v>
       </c>
-      <c r="S27" t="str">
-        <f t="shared" si="6"/>
+      <c r="W27" t="str">
+        <f t="shared" si="7"/>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55</v>
       </c>
-      <c r="U27" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y27" t="str">
+        <f>Y26&amp;", "&amp;K27</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91, 82, 70, 54</v>
       </c>
-      <c r="W27" t="str">
-        <f t="shared" si="8"/>
+      <c r="AA27" t="str">
+        <f>AA26&amp;", "&amp;M27</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K28">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M28">
         <v>24</v>
       </c>
-      <c r="W28" t="str">
-        <f t="shared" ref="W28:W91" si="10">W27&amp;", "&amp;K28</f>
+      <c r="AA28" t="str">
+        <f t="shared" ref="AA28:AA91" si="11">AA27&amp;", "&amp;M28</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K29">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M29">
         <v>25</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA29" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>26</v>
+      </c>
+      <c r="O30" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA30" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>27</v>
+      </c>
+      <c r="O31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA31" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>28</v>
+      </c>
+      <c r="AA32" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28</v>
+      </c>
+    </row>
+    <row r="33" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>29</v>
+      </c>
+      <c r="O33" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA33" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29</v>
+      </c>
+    </row>
+    <row r="34" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>30</v>
+      </c>
+      <c r="O34" t="s">
         <v>156</v>
       </c>
-      <c r="W29" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K30">
-        <v>26</v>
-      </c>
-      <c r="M30" t="s">
+      <c r="AA34" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30</v>
+      </c>
+    </row>
+    <row r="35" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>31</v>
+      </c>
+      <c r="O35" t="s">
         <v>157</v>
       </c>
-      <c r="W30" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K31">
-        <v>27</v>
-      </c>
-      <c r="M31" t="s">
+      <c r="AA35" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31</v>
+      </c>
+    </row>
+    <row r="36" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>32</v>
+      </c>
+      <c r="AA36" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32</v>
+      </c>
+    </row>
+    <row r="37" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>33</v>
+      </c>
+      <c r="O37" t="s">
         <v>158</v>
       </c>
-      <c r="W31" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K32">
-        <v>28</v>
-      </c>
-      <c r="M32" t="s">
+      <c r="AA37" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33</v>
+      </c>
+    </row>
+    <row r="38" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>34</v>
+      </c>
+      <c r="O38" t="s">
         <v>159</v>
       </c>
-      <c r="W32" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28</v>
-      </c>
-    </row>
-    <row r="33" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K33">
-        <v>29</v>
-      </c>
-      <c r="W33" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29</v>
-      </c>
-    </row>
-    <row r="34" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K34">
-        <v>30</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="AA38" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34</v>
+      </c>
+    </row>
+    <row r="39" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>35</v>
+      </c>
+      <c r="O39" t="s">
         <v>160</v>
       </c>
-      <c r="W34" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30</v>
-      </c>
-    </row>
-    <row r="35" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K35">
-        <v>31</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="AA39" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35</v>
+      </c>
+    </row>
+    <row r="40" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>36</v>
+      </c>
+      <c r="O40" t="s">
         <v>161</v>
       </c>
-      <c r="W35" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31</v>
-      </c>
-    </row>
-    <row r="36" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K36">
-        <v>32</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="AA40" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36</v>
+      </c>
+    </row>
+    <row r="41" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>37</v>
+      </c>
+      <c r="AA41" t="str">
+        <f t="shared" si="11"/>
+        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37</v>
+      </c>
+    </row>
+    <row r="42" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>38</v>
+      </c>
+      <c r="O42" t="s">
         <v>162</v>
       </c>
-      <c r="W36" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32</v>
-      </c>
-    </row>
-    <row r="37" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K37">
-        <v>33</v>
-      </c>
-      <c r="M37" t="s">
-        <v>163</v>
-      </c>
-      <c r="W37" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33</v>
-      </c>
-    </row>
-    <row r="38" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K38">
-        <v>34</v>
-      </c>
-      <c r="W38" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34</v>
-      </c>
-    </row>
-    <row r="39" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K39">
-        <v>35</v>
-      </c>
-      <c r="M39" t="s">
-        <v>164</v>
-      </c>
-      <c r="W39" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35</v>
-      </c>
-    </row>
-    <row r="40" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K40">
-        <v>36</v>
-      </c>
-      <c r="W40" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36</v>
-      </c>
-    </row>
-    <row r="41" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K41">
-        <v>37</v>
-      </c>
-      <c r="W41" t="str">
-        <f t="shared" si="10"/>
-        <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37</v>
-      </c>
-    </row>
-    <row r="42" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K42">
-        <v>38</v>
-      </c>
-      <c r="W42" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA42" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38</v>
       </c>
     </row>
-    <row r="43" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K43">
+    <row r="43" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M43">
         <v>39</v>
       </c>
-      <c r="W43" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA43" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39</v>
       </c>
     </row>
-    <row r="44" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K44">
+    <row r="44" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M44">
         <v>40</v>
       </c>
-      <c r="W44" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA44" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40</v>
       </c>
     </row>
-    <row r="45" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K45">
+    <row r="45" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M45">
         <v>41</v>
       </c>
-      <c r="W45" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA45" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41</v>
       </c>
     </row>
-    <row r="46" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K46">
+    <row r="46" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M46">
         <v>42</v>
       </c>
-      <c r="W46" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA46" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42</v>
       </c>
     </row>
-    <row r="47" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K47">
+    <row r="47" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M47">
         <v>43</v>
       </c>
-      <c r="W47" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA47" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43</v>
       </c>
     </row>
-    <row r="48" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K48">
+    <row r="48" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M48">
         <v>44</v>
       </c>
-      <c r="W48" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA48" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44</v>
       </c>
     </row>
-    <row r="49" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K49">
+    <row r="49" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M49">
         <v>45</v>
       </c>
-      <c r="W49" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA49" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45</v>
       </c>
     </row>
-    <row r="50" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K50">
+    <row r="50" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M50">
         <v>46</v>
       </c>
-      <c r="W50" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA50" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46</v>
       </c>
     </row>
-    <row r="51" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K51">
+    <row r="51" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M51">
         <v>47</v>
       </c>
-      <c r="W51" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA51" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47</v>
       </c>
     </row>
-    <row r="52" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K52">
+    <row r="52" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M52">
         <v>48</v>
       </c>
-      <c r="W52" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA52" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48</v>
       </c>
     </row>
-    <row r="53" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K53">
+    <row r="53" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M53">
         <v>49</v>
       </c>
-      <c r="W53" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA53" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49</v>
       </c>
     </row>
-    <row r="54" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K54">
+    <row r="54" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M54">
         <v>50</v>
       </c>
-      <c r="W54" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA54" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50</v>
       </c>
     </row>
-    <row r="55" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K55">
+    <row r="55" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M55">
         <v>51</v>
       </c>
-      <c r="W55" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA55" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51</v>
       </c>
     </row>
-    <row r="56" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K56">
+    <row r="56" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M56">
         <v>52</v>
       </c>
-      <c r="W56" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA56" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52</v>
       </c>
     </row>
-    <row r="57" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K57">
+    <row r="57" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M57">
         <v>53</v>
       </c>
-      <c r="W57" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA57" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53</v>
       </c>
     </row>
-    <row r="58" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K58">
+    <row r="58" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M58">
         <v>54</v>
       </c>
-      <c r="W58" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA58" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54</v>
       </c>
     </row>
-    <row r="59" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K59">
+    <row r="59" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M59">
         <v>55</v>
       </c>
-      <c r="W59" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA59" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55</v>
       </c>
     </row>
-    <row r="60" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K60">
+    <row r="60" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M60">
         <v>56</v>
       </c>
-      <c r="W60" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA60" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56</v>
       </c>
     </row>
-    <row r="61" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K61">
+    <row r="61" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M61">
         <v>57</v>
       </c>
-      <c r="W61" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA61" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57</v>
       </c>
     </row>
-    <row r="62" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K62">
+    <row r="62" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M62">
         <v>58</v>
       </c>
-      <c r="W62" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA62" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58</v>
       </c>
     </row>
-    <row r="63" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K63">
+    <row r="63" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M63">
         <v>59</v>
       </c>
-      <c r="W63" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA63" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59</v>
       </c>
     </row>
-    <row r="64" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K64">
+    <row r="64" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M64">
         <v>60</v>
       </c>
-      <c r="W64" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA64" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60</v>
       </c>
     </row>
-    <row r="65" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K65">
+    <row r="65" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M65">
         <v>61</v>
       </c>
-      <c r="W65" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA65" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61</v>
       </c>
     </row>
-    <row r="66" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K66">
+    <row r="66" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M66">
         <v>62</v>
       </c>
-      <c r="W66" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA66" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62</v>
       </c>
     </row>
-    <row r="67" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K67">
+    <row r="67" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M67">
         <v>63</v>
       </c>
-      <c r="W67" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA67" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63</v>
       </c>
     </row>
-    <row r="68" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K68">
+    <row r="68" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M68">
         <v>64</v>
       </c>
-      <c r="W68" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA68" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64</v>
       </c>
     </row>
-    <row r="69" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K69">
+    <row r="69" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M69">
         <v>65</v>
       </c>
-      <c r="W69" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA69" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65</v>
       </c>
     </row>
-    <row r="70" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K70">
+    <row r="70" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M70">
         <v>66</v>
       </c>
-      <c r="W70" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA70" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66</v>
       </c>
     </row>
-    <row r="71" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K71">
+    <row r="71" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M71">
         <v>67</v>
       </c>
-      <c r="W71" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA71" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67</v>
       </c>
     </row>
-    <row r="72" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K72">
+    <row r="72" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M72">
         <v>68</v>
       </c>
-      <c r="W72" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA72" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68</v>
       </c>
     </row>
-    <row r="73" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K73">
+    <row r="73" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M73">
         <v>69</v>
       </c>
-      <c r="W73" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA73" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69</v>
       </c>
     </row>
-    <row r="74" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K74">
+    <row r="74" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M74">
         <v>70</v>
       </c>
-      <c r="W74" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA74" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70</v>
       </c>
     </row>
-    <row r="75" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K75">
+    <row r="75" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M75">
         <v>71</v>
       </c>
-      <c r="W75" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA75" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71</v>
       </c>
     </row>
-    <row r="76" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K76">
+    <row r="76" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M76">
         <v>72</v>
       </c>
-      <c r="W76" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA76" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72</v>
       </c>
     </row>
-    <row r="77" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K77">
+    <row r="77" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M77">
         <v>73</v>
       </c>
-      <c r="W77" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA77" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73</v>
       </c>
     </row>
-    <row r="78" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K78">
+    <row r="78" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M78">
         <v>74</v>
       </c>
-      <c r="W78" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA78" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74</v>
       </c>
     </row>
-    <row r="79" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K79">
+    <row r="79" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M79">
         <v>75</v>
       </c>
-      <c r="W79" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA79" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75</v>
       </c>
     </row>
-    <row r="80" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K80">
+    <row r="80" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M80">
         <v>76</v>
       </c>
-      <c r="W80" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA80" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76</v>
       </c>
     </row>
-    <row r="81" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K81">
+    <row r="81" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M81">
         <v>77</v>
       </c>
-      <c r="W81" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA81" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77</v>
       </c>
     </row>
-    <row r="82" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K82">
+    <row r="82" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M82">
         <v>78</v>
       </c>
-      <c r="W82" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA82" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78</v>
       </c>
     </row>
-    <row r="83" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K83">
+    <row r="83" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M83">
         <v>79</v>
       </c>
-      <c r="W83" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA83" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79</v>
       </c>
     </row>
-    <row r="84" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K84">
+    <row r="84" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M84">
         <v>80</v>
       </c>
-      <c r="W84" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA84" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80</v>
       </c>
     </row>
-    <row r="85" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K85">
+    <row r="85" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M85">
         <v>81</v>
       </c>
-      <c r="W85" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA85" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81</v>
       </c>
     </row>
-    <row r="86" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K86">
+    <row r="86" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M86">
         <v>82</v>
       </c>
-      <c r="W86" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA86" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82</v>
       </c>
     </row>
-    <row r="87" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K87">
+    <row r="87" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M87">
         <v>83</v>
       </c>
-      <c r="W87" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA87" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83</v>
       </c>
     </row>
-    <row r="88" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K88">
+    <row r="88" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M88">
         <v>84</v>
       </c>
-      <c r="W88" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA88" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84</v>
       </c>
     </row>
-    <row r="89" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K89">
+    <row r="89" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M89">
         <v>85</v>
       </c>
-      <c r="W89" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA89" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85</v>
       </c>
     </row>
-    <row r="90" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K90">
+    <row r="90" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M90">
         <v>86</v>
       </c>
-      <c r="W90" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA90" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86</v>
       </c>
     </row>
-    <row r="91" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K91">
+    <row r="91" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M91">
         <v>87</v>
       </c>
-      <c r="W91" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA91" t="str">
+        <f t="shared" si="11"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87</v>
       </c>
     </row>
-    <row r="92" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K92">
+    <row r="92" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M92">
         <v>88</v>
       </c>
-      <c r="W92" t="str">
-        <f t="shared" ref="W92:W96" si="11">W91&amp;", "&amp;K92</f>
+      <c r="AA92" t="str">
+        <f t="shared" ref="AA92:AA96" si="12">AA91&amp;", "&amp;M92</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88</v>
       </c>
     </row>
-    <row r="93" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K93">
+    <row r="93" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M93">
         <v>89</v>
       </c>
-      <c r="W93" t="str">
-        <f t="shared" si="11"/>
+      <c r="AA93" t="str">
+        <f t="shared" si="12"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89</v>
       </c>
     </row>
-    <row r="94" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K94">
+    <row r="94" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M94">
         <v>90</v>
       </c>
-      <c r="W94" t="str">
-        <f t="shared" si="11"/>
+      <c r="AA94" t="str">
+        <f t="shared" si="12"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90</v>
       </c>
     </row>
-    <row r="95" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K95">
+    <row r="95" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M95">
         <v>91</v>
       </c>
-      <c r="W95" t="str">
-        <f t="shared" si="11"/>
+      <c r="AA95" t="str">
+        <f t="shared" si="12"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91</v>
       </c>
     </row>
-    <row r="96" spans="11:23" x14ac:dyDescent="0.25">
-      <c r="K96">
+    <row r="96" spans="13:27" x14ac:dyDescent="0.25">
+      <c r="M96">
         <v>92</v>
       </c>
-      <c r="W96" t="str">
-        <f t="shared" si="11"/>
+      <c r="AA96" t="str">
+        <f t="shared" si="12"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92</v>
       </c>
     </row>
@@ -11037,10 +11313,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView topLeftCell="H48" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView topLeftCell="H69" workbookViewId="0">
+      <selection activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11987,7 +12263,73 @@
         <v>122</v>
       </c>
     </row>
+    <row r="78" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K78" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K79" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K80" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>5.8</v>
+      </c>
+      <c r="M81">
+        <v>5</v>
+      </c>
+      <c r="N81">
+        <f>L81*M81*1000</f>
+        <v>29000</v>
+      </c>
+      <c r="O81" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K83" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K86" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K89" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="90" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K90" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K78" r:id="rId1"/>
+    <hyperlink ref="K86" r:id="rId2" display="https://smile.amazon.com/RAVPower-32000mAh-Portable-High-Density-Li-Polymer/dp/B06XZ6KSG3/ref=pd_sbs_107_10?_encoding=UTF8&amp;pd_rd_i=B06XZ6KSG3&amp;pd_rd_r=3GSJP7F0DQ588TP9E1E2&amp;pd_rd_w=pZ6TK&amp;pd_rd_wg=o9KlO&amp;psc=1&amp;refRID=3GSJP7F0DQ588TP9E1E2"/>
+    <hyperlink ref="K89" r:id="rId3" tooltip="[Upgraded] Poweradd Pilot Pro3 30000mAh Power Bank (Dual Inputs/4A, 3 Outputs/4.5A) External Battery Pack with High-Speed Smart Charge for iPhone, iPad, Samsung, LG, Nexus and More" display="https://smile.amazon.com/gp/slredirect/picassoRedirect.html/ref=sspa_dk_detail_4?ie=UTF8&amp;adId=A06848401NTNKZNFLGGDG&amp;qualifier=1515303508&amp;id=154144488656348&amp;widgetName=sp_detail&amp;url=%2Fdp%2FB01M5LKV4T%2Fref%3Dsspa_dk_detail_4%3Fpsc%3D1%26pd_rd_i%3DB01M5LKV4T%26pd_rd_wg%3DA6Dsb%26pd_rd_r%3DE4QY1G0ZAFBNGQW3P696%26pd_rd_w%3DaLxyw"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
method to mark adjacent cells
</commit_message>
<xml_diff>
--- a/GraduationCapDesign_2017.xlsx
+++ b/GraduationCapDesign_2017.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="180">
   <si>
     <t>LED count</t>
   </si>
@@ -801,6 +801,9 @@
   </si>
   <si>
     <t>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74, 58, 35 };</t>
+  </si>
+  <si>
+    <t>used</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1147,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1227,6 +1230,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2578,22 +2584,22 @@
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
       <c r="X2" s="35"/>
       <c r="Y2" t="s">
         <v>147</v>
       </c>
-      <c r="Z2" s="39" t="s">
+      <c r="Z2" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
     </row>
     <row r="3" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G3" s="33" t="s">
@@ -9102,22 +9108,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AA96"/>
+  <dimension ref="A2:AK96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="3.85546875" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="11" width="3.85546875" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="15" max="17" width="12.85546875" customWidth="1"/>
+    <col min="1" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="12" width="3.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1"/>
+    <col min="16" max="18" width="12.85546875" customWidth="1"/>
+    <col min="31" max="32" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>151</v>
       </c>
@@ -9127,67 +9134,71 @@
       <c r="C2" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="F2" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="G2" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35">
+      <c r="H2" s="35"/>
+      <c r="I2" s="35">
         <v>2</v>
       </c>
-      <c r="I2" s="35">
-        <v>0</v>
-      </c>
       <c r="J2" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="35">
+        <v>1</v>
+      </c>
+      <c r="L2" s="35">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>155</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="P2" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="Q2" s="38" t="s">
+      <c r="R2" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="S2" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="T2" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="U2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36">
+      <c r="V2" s="36"/>
+      <c r="W2" s="36">
         <v>2</v>
       </c>
-      <c r="W2" s="36">
-        <v>0</v>
-      </c>
       <c r="X2" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="36">
         <v>8</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>-COUNTA(A4:A96)</f>
         <v>-17</v>
@@ -9200,84 +9211,105 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-      <c r="D3">
-        <f>-COUNTA(D4:D96)</f>
-        <v>-12</v>
-      </c>
       <c r="E3">
         <f>-COUNTA(E4:E96)</f>
-        <v>-17</v>
+        <v>-12</v>
       </c>
       <c r="F3">
         <f>-COUNTA(F4:F96)</f>
         <v>-17</v>
       </c>
-      <c r="H3">
-        <f>-COUNTA(H4:H96)</f>
+      <c r="G3">
+        <f>-COUNTA(G4:G96)</f>
         <v>-17</v>
       </c>
       <c r="I3">
         <f>-COUNTA(I4:I96)</f>
-        <v>-24</v>
+        <v>-17</v>
       </c>
       <c r="J3">
         <f>-COUNTA(J4:J96)</f>
-        <v>-15</v>
+        <v>-24</v>
       </c>
       <c r="K3">
         <f>-COUNTA(K4:K96)</f>
+        <v>-15</v>
+      </c>
+      <c r="L3">
+        <f>-COUNTA(L4:L96)</f>
         <v>-24</v>
       </c>
-      <c r="M3">
-        <f>-COUNTA(M4:M96)</f>
+      <c r="N3">
+        <f>-COUNTA(N4:N96)</f>
         <v>-93</v>
       </c>
-      <c r="O3" t="str">
-        <f>"const char ltr_"&amp;O2&amp;"["&amp;1-A3&amp;"] = { "&amp;A3</f>
+      <c r="P3" t="str">
+        <f>"const char ltr_"&amp;P2&amp;"["&amp;1-A3&amp;"] = { "&amp;A3</f>
         <v>const char ltr_P[18] = { -17</v>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:Q3" si="1">"const char ltr_"&amp;P2&amp;"["&amp;1-B3&amp;"] = { "&amp;B3</f>
+      <c r="Q3" t="str">
+        <f>"const char ltr_"&amp;Q2&amp;"["&amp;1-B3&amp;"] = { "&amp;B3</f>
         <v>const char ltr_L[11] = { -10</v>
       </c>
-      <c r="Q3" t="str">
-        <f t="shared" si="1"/>
+      <c r="R3" t="str">
+        <f>"const char ltr_"&amp;R2&amp;"["&amp;1-C3&amp;"] = { "&amp;C3</f>
         <v>const char ltr_Y[13] = { -12</v>
-      </c>
-      <c r="R3" t="str">
-        <f>"const char ltr_"&amp;R2&amp;"["&amp;1-D3&amp;"] = { "&amp;D3</f>
-        <v>const char ltr_T[13] = { -12</v>
       </c>
       <c r="S3" t="str">
         <f>"const char ltr_"&amp;S2&amp;"["&amp;1-E3&amp;"] = { "&amp;E3</f>
-        <v>const char ltr_H[18] = { -17</v>
+        <v>const char ltr_T[13] = { -12</v>
       </c>
       <c r="T3" t="str">
         <f>"const char ltr_"&amp;T2&amp;"["&amp;1-F3&amp;"] = { "&amp;F3</f>
+        <v>const char ltr_H[18] = { -17</v>
+      </c>
+      <c r="U3" t="str">
+        <f>"const char ltr_"&amp;U2&amp;"["&amp;1-G3&amp;"] = { "&amp;G3</f>
         <v>const char ltr_S[18] = { -17</v>
-      </c>
-      <c r="V3" t="str">
-        <f>"const char ltr_"&amp;V2&amp;"["&amp;1-H3&amp;"] = { "&amp;H3</f>
-        <v>const char ltr_2[18] = { -17</v>
       </c>
       <c r="W3" t="str">
         <f>"const char ltr_"&amp;W2&amp;"["&amp;1-I3&amp;"] = { "&amp;I3</f>
-        <v>const char ltr_0[25] = { -24</v>
+        <v>const char ltr_2[18] = { -17</v>
       </c>
       <c r="X3" t="str">
         <f>"const char ltr_"&amp;X2&amp;"["&amp;1-J3&amp;"] = { "&amp;J3</f>
-        <v>const char ltr_1[16] = { -15</v>
+        <v>const char ltr_0[25] = { -24</v>
       </c>
       <c r="Y3" t="str">
         <f>"const char ltr_"&amp;Y2&amp;"["&amp;1-K3&amp;"] = { "&amp;K3</f>
+        <v>const char ltr_1[16] = { -15</v>
+      </c>
+      <c r="Z3" t="str">
+        <f>"const char ltr_"&amp;Z2&amp;"["&amp;1-L3&amp;"] = { "&amp;L3</f>
         <v>const char ltr_8[25] = { -24</v>
       </c>
-      <c r="AA3" t="str">
-        <f>"const char ltr_"&amp;AA2&amp;"["&amp;1-M3&amp;"] = { "&amp;M3</f>
+      <c r="AB3" t="str">
+        <f>"const char ltr_"&amp;AB2&amp;"["&amp;1-N3&amp;"] = { "&amp;N3</f>
         <v>const char ltr_all[94] = { -93</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE3">
+        <v>32</v>
+      </c>
+      <c r="AF3">
+        <v>31</v>
+      </c>
+      <c r="AG3">
+        <v>55</v>
+      </c>
+      <c r="AH3">
+        <v>56</v>
+      </c>
+      <c r="AI3">
+        <v>33</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>81</v>
       </c>
@@ -9287,76 +9319,91 @@
       <c r="C4">
         <v>78</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>53</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>54</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>34</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>53</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>32</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>53</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>54</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="str">
-        <f>O3&amp;", "&amp;A4</f>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="str">
+        <f>P3&amp;", "&amp;A4</f>
         <v>const char ltr_P[18] = { -17, 81</v>
       </c>
-      <c r="P4" t="str">
-        <f t="shared" ref="P4:Q15" si="2">P3&amp;", "&amp;B4</f>
+      <c r="Q4" t="str">
+        <f>Q3&amp;", "&amp;B4</f>
         <v>const char ltr_L[11] = { -10, 54</v>
       </c>
-      <c r="Q4" t="str">
-        <f t="shared" si="2"/>
+      <c r="R4" t="str">
+        <f>R3&amp;", "&amp;C4</f>
         <v>const char ltr_Y[13] = { -12, 78</v>
       </c>
-      <c r="R4" t="str">
-        <f t="shared" ref="R4:R15" si="3">R3&amp;", "&amp;D4</f>
+      <c r="S4" t="str">
+        <f>S3&amp;", "&amp;E4</f>
         <v>const char ltr_T[13] = { -12, 53</v>
       </c>
-      <c r="S4" t="str">
-        <f t="shared" ref="S4:S20" si="4">S3&amp;", "&amp;E4</f>
+      <c r="T4" t="str">
+        <f>T3&amp;", "&amp;F4</f>
         <v>const char ltr_H[18] = { -17, 54</v>
       </c>
-      <c r="T4" t="str">
-        <f t="shared" ref="T4:T20" si="5">T3&amp;", "&amp;F4</f>
+      <c r="U4" t="str">
+        <f>U3&amp;", "&amp;G4</f>
         <v>const char ltr_S[18] = { -17, 34</v>
       </c>
-      <c r="V4" t="str">
-        <f t="shared" ref="V4:V20" si="6">V3&amp;", "&amp;H4</f>
+      <c r="W4" t="str">
+        <f>W3&amp;", "&amp;I4</f>
         <v>const char ltr_2[18] = { -17, 53</v>
       </c>
-      <c r="W4" t="str">
-        <f t="shared" ref="W4:W27" si="7">W3&amp;", "&amp;I4</f>
+      <c r="X4" t="str">
+        <f>X3&amp;", "&amp;J4</f>
         <v>const char ltr_0[25] = { -24, 32</v>
-      </c>
-      <c r="X4" t="str">
-        <f t="shared" ref="X4:X18" si="8">X3&amp;", "&amp;J4</f>
-        <v>const char ltr_1[16] = { -15, 53</v>
       </c>
       <c r="Y4" t="str">
         <f>Y3&amp;", "&amp;K4</f>
+        <v>const char ltr_1[16] = { -15, 53</v>
+      </c>
+      <c r="Z4" t="str">
+        <f>Z3&amp;", "&amp;L4</f>
         <v>const char ltr_8[25] = { -24, 54</v>
       </c>
-      <c r="AA4" t="str">
-        <f>AA3&amp;", "&amp;M4</f>
+      <c r="AB4" t="str">
+        <f t="shared" ref="AB4:AB27" si="1">AB3&amp;", "&amp;N4</f>
         <v>const char ltr_all[94] = { -93, 0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE4">
+        <v>33</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>32</v>
+      </c>
+      <c r="AH4">
+        <v>57</v>
+      </c>
+      <c r="AI4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>82</v>
       </c>
@@ -9366,76 +9413,94 @@
       <c r="C5">
         <v>64</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>71</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>70</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>33</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>54</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>33</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>54</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>55</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" ref="O5:O11" si="9">O4&amp;", "&amp;A5</f>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="str">
+        <f>P4&amp;", "&amp;A5</f>
         <v>const char ltr_P[18] = { -17, 81, 82</v>
       </c>
-      <c r="P5" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q5" t="str">
+        <f>Q4&amp;", "&amp;B5</f>
         <v>const char ltr_L[11] = { -10, 54, 70</v>
       </c>
-      <c r="Q5" t="str">
-        <f t="shared" si="2"/>
+      <c r="R5" t="str">
+        <f>R4&amp;", "&amp;C5</f>
         <v>const char ltr_Y[13] = { -12, 78, 64</v>
       </c>
-      <c r="R5" t="str">
-        <f t="shared" si="3"/>
+      <c r="S5" t="str">
+        <f>S4&amp;", "&amp;E5</f>
         <v>const char ltr_T[13] = { -12, 53, 71</v>
       </c>
-      <c r="S5" t="str">
-        <f t="shared" si="4"/>
+      <c r="T5" t="str">
+        <f>T4&amp;", "&amp;F5</f>
         <v>const char ltr_H[18] = { -17, 54, 70</v>
       </c>
-      <c r="T5" t="str">
-        <f t="shared" si="5"/>
+      <c r="U5" t="str">
+        <f>U4&amp;", "&amp;G5</f>
         <v>const char ltr_S[18] = { -17, 34, 33</v>
       </c>
-      <c r="V5" t="str">
-        <f t="shared" si="6"/>
+      <c r="W5" t="str">
+        <f>W4&amp;", "&amp;I5</f>
         <v>const char ltr_2[18] = { -17, 53, 54</v>
       </c>
-      <c r="W5" t="str">
-        <f t="shared" si="7"/>
+      <c r="X5" t="str">
+        <f>X4&amp;", "&amp;J5</f>
         <v>const char ltr_0[25] = { -24, 32, 33</v>
-      </c>
-      <c r="X5" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54</v>
       </c>
       <c r="Y5" t="str">
         <f>Y4&amp;", "&amp;K5</f>
+        <v>const char ltr_1[16] = { -15, 53, 54</v>
+      </c>
+      <c r="Z5" t="str">
+        <f>Z4&amp;", "&amp;L5</f>
         <v>const char ltr_8[25] = { -24, 54, 55</v>
       </c>
-      <c r="AA5" t="str">
-        <f>AA4&amp;", "&amp;M5</f>
+      <c r="AB5" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE5">
+        <v>34</v>
+      </c>
+      <c r="AF5">
+        <v>2</v>
+      </c>
+      <c r="AG5">
+        <v>33</v>
+      </c>
+      <c r="AH5">
+        <v>47</v>
+      </c>
+      <c r="AI5">
+        <v>35</v>
+      </c>
+      <c r="AJ5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>70</v>
       </c>
@@ -9445,76 +9510,94 @@
       <c r="C6">
         <v>44</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>56</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>82</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>32</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>55</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>34</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>55</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>32</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>2</v>
       </c>
-      <c r="O6" t="str">
-        <f t="shared" si="9"/>
+      <c r="P6" t="str">
+        <f>P5&amp;", "&amp;A6</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70</v>
       </c>
-      <c r="P6" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q6" t="str">
+        <f>Q5&amp;", "&amp;B6</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82</v>
       </c>
-      <c r="Q6" t="str">
-        <f t="shared" si="2"/>
+      <c r="R6" t="str">
+        <f>R5&amp;", "&amp;C6</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44</v>
       </c>
-      <c r="R6" t="str">
-        <f t="shared" si="3"/>
+      <c r="S6" t="str">
+        <f>S5&amp;", "&amp;E6</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56</v>
       </c>
-      <c r="S6" t="str">
-        <f t="shared" si="4"/>
+      <c r="T6" t="str">
+        <f>T5&amp;", "&amp;F6</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82</v>
       </c>
-      <c r="T6" t="str">
-        <f t="shared" si="5"/>
+      <c r="U6" t="str">
+        <f>U5&amp;", "&amp;G6</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32</v>
       </c>
-      <c r="V6" t="str">
-        <f t="shared" si="6"/>
+      <c r="W6" t="str">
+        <f>W5&amp;", "&amp;I6</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55</v>
       </c>
-      <c r="W6" t="str">
-        <f t="shared" si="7"/>
+      <c r="X6" t="str">
+        <f>X5&amp;", "&amp;J6</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55</v>
       </c>
       <c r="Y6" t="str">
         <f>Y5&amp;", "&amp;K6</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55</v>
+      </c>
+      <c r="Z6" t="str">
+        <f>Z5&amp;", "&amp;L6</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32</v>
       </c>
-      <c r="AA6" t="str">
-        <f>AA5&amp;", "&amp;M6</f>
+      <c r="AB6" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE6">
+        <v>35</v>
+      </c>
+      <c r="AF6">
+        <v>3</v>
+      </c>
+      <c r="AG6">
+        <v>34</v>
+      </c>
+      <c r="AH6">
+        <v>58</v>
+      </c>
+      <c r="AI6">
+        <v>36</v>
+      </c>
+      <c r="AJ6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>54</v>
       </c>
@@ -9524,76 +9607,94 @@
       <c r="C7">
         <v>53</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>57</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>81</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>55</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>32</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>35</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>32</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>33</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>3</v>
       </c>
-      <c r="O7" t="str">
-        <f t="shared" si="9"/>
+      <c r="P7" t="str">
+        <f>P6&amp;", "&amp;A7</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54</v>
       </c>
-      <c r="P7" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q7" t="str">
+        <f>Q6&amp;", "&amp;B7</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81</v>
       </c>
-      <c r="Q7" t="str">
-        <f t="shared" si="2"/>
+      <c r="R7" t="str">
+        <f>R6&amp;", "&amp;C7</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53</v>
       </c>
-      <c r="R7" t="str">
-        <f t="shared" si="3"/>
+      <c r="S7" t="str">
+        <f>S6&amp;", "&amp;E7</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57</v>
       </c>
-      <c r="S7" t="str">
-        <f t="shared" si="4"/>
+      <c r="T7" t="str">
+        <f>T6&amp;", "&amp;F7</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81</v>
       </c>
-      <c r="T7" t="str">
-        <f t="shared" si="5"/>
+      <c r="U7" t="str">
+        <f>U6&amp;", "&amp;G7</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55</v>
       </c>
-      <c r="V7" t="str">
-        <f t="shared" si="6"/>
+      <c r="W7" t="str">
+        <f>W6&amp;", "&amp;I7</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32</v>
       </c>
-      <c r="W7" t="str">
-        <f t="shared" si="7"/>
+      <c r="X7" t="str">
+        <f>X6&amp;", "&amp;J7</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35</v>
-      </c>
-      <c r="X7" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32</v>
       </c>
       <c r="Y7" t="str">
         <f>Y6&amp;", "&amp;K7</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32</v>
+      </c>
+      <c r="Z7" t="str">
+        <f>Z6&amp;", "&amp;L7</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33</v>
       </c>
-      <c r="AA7" t="str">
-        <f>AA6&amp;", "&amp;M7</f>
+      <c r="AB7" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE7">
+        <v>36</v>
+      </c>
+      <c r="AF7">
+        <v>35</v>
+      </c>
+      <c r="AG7">
+        <v>59</v>
+      </c>
+      <c r="AH7">
+        <v>37</v>
+      </c>
+      <c r="AI7">
+        <v>6</v>
+      </c>
+      <c r="AJ7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>55</v>
       </c>
@@ -9603,76 +9704,97 @@
       <c r="C8">
         <v>70</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>35</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>80</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>54</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>33</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>36</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>56</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>34</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>4</v>
       </c>
-      <c r="O8" t="str">
-        <f t="shared" si="9"/>
+      <c r="P8" t="str">
+        <f>P7&amp;", "&amp;A8</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55</v>
       </c>
-      <c r="P8" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q8" t="str">
+        <f>Q7&amp;", "&amp;B8</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80</v>
       </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="2"/>
+      <c r="R8" t="str">
+        <f>R7&amp;", "&amp;C8</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70</v>
       </c>
-      <c r="R8" t="str">
-        <f t="shared" si="3"/>
+      <c r="S8" t="str">
+        <f>S7&amp;", "&amp;E8</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35</v>
       </c>
-      <c r="S8" t="str">
-        <f t="shared" si="4"/>
+      <c r="T8" t="str">
+        <f>T7&amp;", "&amp;F8</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80</v>
       </c>
-      <c r="T8" t="str">
-        <f t="shared" si="5"/>
+      <c r="U8" t="str">
+        <f>U7&amp;", "&amp;G8</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54</v>
       </c>
-      <c r="V8" t="str">
-        <f t="shared" si="6"/>
+      <c r="W8" t="str">
+        <f>W7&amp;", "&amp;I8</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33</v>
       </c>
-      <c r="W8" t="str">
-        <f t="shared" si="7"/>
+      <c r="X8" t="str">
+        <f>X7&amp;", "&amp;J8</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56</v>
       </c>
       <c r="Y8" t="str">
         <f>Y7&amp;", "&amp;K8</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56</v>
+      </c>
+      <c r="Z8" t="str">
+        <f>Z7&amp;", "&amp;L8</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34</v>
       </c>
-      <c r="AA8" t="str">
-        <f>AA7&amp;", "&amp;M8</f>
+      <c r="AB8" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE8">
+        <v>37</v>
+      </c>
+      <c r="AF8">
+        <v>36</v>
+      </c>
+      <c r="AG8">
+        <v>59</v>
+      </c>
+      <c r="AH8">
+        <v>38</v>
+      </c>
+      <c r="AI8">
+        <v>7</v>
+      </c>
+      <c r="AJ8">
+        <v>6</v>
+      </c>
+      <c r="AK8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32</v>
       </c>
@@ -9682,76 +9804,79 @@
       <c r="C9">
         <v>82</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>72</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>66</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>70</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>34</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>37</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>72</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>58</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>5</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" si="9"/>
+      <c r="P9" t="str">
+        <f>P8&amp;", "&amp;A9</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32</v>
       </c>
-      <c r="P9" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q9" t="str">
+        <f>Q8&amp;", "&amp;B9</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66</v>
       </c>
-      <c r="Q9" t="str">
-        <f t="shared" si="2"/>
+      <c r="R9" t="str">
+        <f>R8&amp;", "&amp;C9</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82</v>
       </c>
-      <c r="R9" t="str">
-        <f t="shared" si="3"/>
+      <c r="S9" t="str">
+        <f>S8&amp;", "&amp;E9</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72</v>
       </c>
-      <c r="S9" t="str">
-        <f t="shared" si="4"/>
+      <c r="T9" t="str">
+        <f>T8&amp;", "&amp;F9</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66</v>
       </c>
-      <c r="T9" t="str">
-        <f t="shared" si="5"/>
+      <c r="U9" t="str">
+        <f>U8&amp;", "&amp;G9</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70</v>
       </c>
-      <c r="V9" t="str">
-        <f t="shared" si="6"/>
+      <c r="W9" t="str">
+        <f>W8&amp;", "&amp;I9</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34</v>
       </c>
-      <c r="W9" t="str">
-        <f t="shared" si="7"/>
+      <c r="X9" t="str">
+        <f>X8&amp;", "&amp;J9</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37</v>
-      </c>
-      <c r="X9" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72</v>
       </c>
       <c r="Y9" t="str">
         <f>Y8&amp;", "&amp;K9</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72</v>
+      </c>
+      <c r="Z9" t="str">
+        <f>Z8&amp;", "&amp;L9</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58</v>
       </c>
-      <c r="AA9" t="str">
-        <f>AA8&amp;", "&amp;M9</f>
+      <c r="AB9" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>33</v>
       </c>
@@ -9761,76 +9886,79 @@
       <c r="C10">
         <v>90</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>84</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>46</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>82</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>35</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>38</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>84</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>74</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>6</v>
       </c>
-      <c r="O10" t="str">
-        <f t="shared" si="9"/>
+      <c r="P10" t="str">
+        <f>P9&amp;", "&amp;A10</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33</v>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q10" t="str">
+        <f>Q9&amp;", "&amp;B10</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65</v>
       </c>
-      <c r="Q10" t="str">
-        <f t="shared" si="2"/>
+      <c r="R10" t="str">
+        <f>R9&amp;", "&amp;C10</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90</v>
       </c>
-      <c r="R10" t="str">
-        <f t="shared" si="3"/>
+      <c r="S10" t="str">
+        <f>S9&amp;", "&amp;E10</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84</v>
       </c>
-      <c r="S10" t="str">
-        <f t="shared" si="4"/>
+      <c r="T10" t="str">
+        <f>T9&amp;", "&amp;F10</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46</v>
       </c>
-      <c r="T10" t="str">
-        <f t="shared" si="5"/>
+      <c r="U10" t="str">
+        <f>U9&amp;", "&amp;G10</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82</v>
       </c>
-      <c r="V10" t="str">
-        <f t="shared" si="6"/>
+      <c r="W10" t="str">
+        <f>W9&amp;", "&amp;I10</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35</v>
       </c>
-      <c r="W10" t="str">
-        <f t="shared" si="7"/>
+      <c r="X10" t="str">
+        <f>X9&amp;", "&amp;J10</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38</v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84</v>
       </c>
       <c r="Y10" t="str">
         <f>Y9&amp;", "&amp;K10</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84</v>
+      </c>
+      <c r="Z10" t="str">
+        <f>Z9&amp;", "&amp;L10</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74</v>
       </c>
-      <c r="AA10" t="str">
-        <f>AA9&amp;", "&amp;M10</f>
+      <c r="AB10" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
@@ -9840,76 +9968,79 @@
       <c r="C11">
         <v>88</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>92</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>34</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>91</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>58</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>39</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>92</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>85</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>7</v>
       </c>
-      <c r="O11" t="str">
-        <f t="shared" si="9"/>
+      <c r="P11" t="str">
+        <f>P10&amp;", "&amp;A11</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34</v>
       </c>
-      <c r="P11" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q11" t="str">
+        <f>Q10&amp;", "&amp;B11</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64</v>
       </c>
-      <c r="Q11" t="str">
-        <f t="shared" si="2"/>
+      <c r="R11" t="str">
+        <f>R10&amp;", "&amp;C11</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88</v>
       </c>
-      <c r="R11" t="str">
-        <f t="shared" si="3"/>
+      <c r="S11" t="str">
+        <f>S10&amp;", "&amp;E11</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92</v>
       </c>
-      <c r="S11" t="str">
-        <f t="shared" si="4"/>
+      <c r="T11" t="str">
+        <f>T10&amp;", "&amp;F11</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34</v>
       </c>
-      <c r="T11" t="str">
-        <f t="shared" si="5"/>
+      <c r="U11" t="str">
+        <f>U10&amp;", "&amp;G11</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91</v>
       </c>
-      <c r="V11" t="str">
-        <f t="shared" si="6"/>
+      <c r="W11" t="str">
+        <f>W10&amp;", "&amp;I11</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58</v>
       </c>
-      <c r="W11" t="str">
-        <f t="shared" si="7"/>
+      <c r="X11" t="str">
+        <f>X10&amp;", "&amp;J11</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39</v>
-      </c>
-      <c r="X11" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92</v>
       </c>
       <c r="Y11" t="str">
         <f>Y10&amp;", "&amp;K11</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92</v>
+      </c>
+      <c r="Z11" t="str">
+        <f>Z10&amp;", "&amp;L11</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85</v>
       </c>
-      <c r="AA11" t="str">
-        <f>AA10&amp;", "&amp;M11</f>
+      <c r="AB11" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
@@ -9919,76 +10050,79 @@
       <c r="C12">
         <v>86</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>88</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>58</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>92</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>85</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>40</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>88</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>92</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>8</v>
       </c>
-      <c r="O12" t="str">
-        <f t="shared" ref="O12:O20" si="10">O11&amp;", "&amp;A13</f>
+      <c r="P12" t="str">
+        <f>P11&amp;", "&amp;A13</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59</v>
       </c>
-      <c r="P12" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q12" t="str">
+        <f>Q11&amp;", "&amp;B12</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64, 63</v>
       </c>
-      <c r="Q12" t="str">
-        <f t="shared" si="2"/>
+      <c r="R12" t="str">
+        <f>R11&amp;", "&amp;C12</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86</v>
       </c>
-      <c r="R12" t="str">
-        <f t="shared" si="3"/>
+      <c r="S12" t="str">
+        <f>S11&amp;", "&amp;E12</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88</v>
       </c>
-      <c r="S12" t="str">
-        <f t="shared" si="4"/>
+      <c r="T12" t="str">
+        <f>T11&amp;", "&amp;F12</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58</v>
       </c>
-      <c r="T12" t="str">
-        <f t="shared" si="5"/>
+      <c r="U12" t="str">
+        <f>U11&amp;", "&amp;G12</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92</v>
       </c>
-      <c r="V12" t="str">
-        <f t="shared" si="6"/>
+      <c r="W12" t="str">
+        <f>W11&amp;", "&amp;I12</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85</v>
       </c>
-      <c r="W12" t="str">
-        <f t="shared" si="7"/>
+      <c r="X12" t="str">
+        <f>X11&amp;", "&amp;J12</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40</v>
-      </c>
-      <c r="X12" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88</v>
       </c>
       <c r="Y12" t="str">
         <f>Y11&amp;", "&amp;K12</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88</v>
+      </c>
+      <c r="Z12" t="str">
+        <f>Z11&amp;", "&amp;L12</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92</v>
       </c>
-      <c r="AA12" t="str">
-        <f>AA11&amp;", "&amp;M12</f>
+      <c r="AB12" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59</v>
       </c>
@@ -9998,1313 +10132,1433 @@
       <c r="C13">
         <v>74</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>78</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>74</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>87</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>92</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>41</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>78</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>89</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>9</v>
       </c>
-      <c r="O13" t="str">
-        <f t="shared" si="10"/>
+      <c r="P13" t="str">
+        <f>P12&amp;", "&amp;A14</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75</v>
       </c>
-      <c r="P13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q13" t="str">
+        <f>Q12&amp;", "&amp;B13</f>
         <v>const char ltr_L[11] = { -10, 54, 70, 82, 81, 80, 66, 65, 64, 63, 41</v>
       </c>
-      <c r="Q13" t="str">
-        <f t="shared" si="2"/>
+      <c r="R13" t="str">
+        <f>R12&amp;", "&amp;C13</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74</v>
       </c>
-      <c r="R13" t="str">
-        <f t="shared" si="3"/>
+      <c r="S13" t="str">
+        <f>S12&amp;", "&amp;E13</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78</v>
       </c>
-      <c r="S13" t="str">
-        <f t="shared" si="4"/>
+      <c r="T13" t="str">
+        <f>T12&amp;", "&amp;F13</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74</v>
       </c>
-      <c r="T13" t="str">
-        <f t="shared" si="5"/>
+      <c r="U13" t="str">
+        <f>U12&amp;", "&amp;G13</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87</v>
       </c>
-      <c r="V13" t="str">
-        <f t="shared" si="6"/>
+      <c r="W13" t="str">
+        <f>W12&amp;", "&amp;I13</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92</v>
       </c>
-      <c r="W13" t="str">
-        <f t="shared" si="7"/>
+      <c r="X13" t="str">
+        <f>X12&amp;", "&amp;J13</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41</v>
-      </c>
-      <c r="X13" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78</v>
       </c>
       <c r="Y13" t="str">
         <f>Y12&amp;", "&amp;K13</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78</v>
+      </c>
+      <c r="Z13" t="str">
+        <f>Z12&amp;", "&amp;L13</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89</v>
       </c>
-      <c r="AA13" t="str">
-        <f>AA12&amp;", "&amp;M13</f>
+      <c r="AB13" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>75</v>
       </c>
       <c r="C14">
         <v>58</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>64</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>75</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>76</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>89</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>42</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>47</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>80</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>10</v>
       </c>
-      <c r="O14" t="str">
-        <f t="shared" si="10"/>
+      <c r="P14" t="str">
+        <f>P13&amp;", "&amp;A15</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86</v>
       </c>
-      <c r="Q14" t="str">
-        <f t="shared" si="2"/>
+      <c r="R14" t="str">
+        <f>R13&amp;", "&amp;C14</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74, 58</v>
       </c>
-      <c r="R14" t="str">
-        <f t="shared" si="3"/>
+      <c r="S14" t="str">
+        <f>S13&amp;", "&amp;E14</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78, 64</v>
       </c>
-      <c r="S14" t="str">
-        <f t="shared" si="4"/>
+      <c r="T14" t="str">
+        <f>T13&amp;", "&amp;F14</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75</v>
       </c>
-      <c r="T14" t="str">
-        <f t="shared" si="5"/>
+      <c r="U14" t="str">
+        <f>U13&amp;", "&amp;G14</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76</v>
       </c>
-      <c r="V14" t="str">
-        <f t="shared" si="6"/>
+      <c r="W14" t="str">
+        <f>W13&amp;", "&amp;I14</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89</v>
       </c>
-      <c r="W14" t="str">
-        <f t="shared" si="7"/>
+      <c r="X14" t="str">
+        <f>X13&amp;", "&amp;J14</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42</v>
-      </c>
-      <c r="X14" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47</v>
       </c>
       <c r="Y14" t="str">
         <f>Y13&amp;", "&amp;K14</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47</v>
+      </c>
+      <c r="Z14" t="str">
+        <f>Z13&amp;", "&amp;L14</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80</v>
       </c>
-      <c r="AA14" t="str">
-        <f>AA13&amp;", "&amp;M14</f>
+      <c r="AB14" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>86</v>
       </c>
       <c r="C15">
         <v>35</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>44</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>76</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>62</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>66</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>43</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>65</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>66</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>11</v>
       </c>
-      <c r="O15" t="str">
-        <f t="shared" si="10"/>
+      <c r="P15" t="str">
+        <f>P14&amp;", "&amp;A16</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92</v>
       </c>
-      <c r="Q15" t="str">
-        <f t="shared" si="2"/>
+      <c r="R15" t="str">
+        <f>R14&amp;", "&amp;C15</f>
         <v>const char ltr_Y[13] = { -12, 78, 64, 44, 53, 70, 82, 90, 88, 86, 74, 58, 35</v>
       </c>
-      <c r="R15" t="str">
-        <f t="shared" si="3"/>
+      <c r="S15" t="str">
+        <f>S14&amp;", "&amp;E15</f>
         <v>const char ltr_T[13] = { -12, 53, 71, 56, 57, 35, 72, 84, 92, 88, 78, 64, 44</v>
       </c>
-      <c r="S15" t="str">
-        <f t="shared" si="4"/>
+      <c r="T15" t="str">
+        <f>T14&amp;", "&amp;F15</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76</v>
       </c>
-      <c r="T15" t="str">
-        <f t="shared" si="5"/>
+      <c r="U15" t="str">
+        <f>U14&amp;", "&amp;G15</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62</v>
       </c>
-      <c r="V15" t="str">
-        <f t="shared" si="6"/>
+      <c r="W15" t="str">
+        <f>W14&amp;", "&amp;I15</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66</v>
       </c>
-      <c r="W15" t="str">
-        <f t="shared" si="7"/>
+      <c r="X15" t="str">
+        <f>X14&amp;", "&amp;J15</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43</v>
-      </c>
-      <c r="X15" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65</v>
       </c>
       <c r="Y15" t="str">
         <f>Y14&amp;", "&amp;K15</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65</v>
+      </c>
+      <c r="Z15" t="str">
+        <f>Z14&amp;", "&amp;L15</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66</v>
       </c>
-      <c r="AA15" t="str">
-        <f>AA14&amp;", "&amp;M15</f>
+      <c r="AB15" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>92</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>62</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>42</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>47</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>44</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>64</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>46</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>12</v>
       </c>
-      <c r="O16" t="str">
-        <f t="shared" si="10"/>
+      <c r="P16" t="str">
+        <f>P15&amp;", "&amp;A17</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90</v>
       </c>
-      <c r="S16" t="str">
-        <f t="shared" si="4"/>
+      <c r="T16" t="str">
+        <f>T15&amp;", "&amp;F16</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62</v>
       </c>
-      <c r="T16" t="str">
-        <f t="shared" si="5"/>
+      <c r="U16" t="str">
+        <f>U15&amp;", "&amp;G16</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42</v>
       </c>
-      <c r="V16" t="str">
-        <f t="shared" si="6"/>
+      <c r="W16" t="str">
+        <f>W15&amp;", "&amp;I16</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47</v>
       </c>
-      <c r="W16" t="str">
-        <f t="shared" si="7"/>
+      <c r="X16" t="str">
+        <f>X15&amp;", "&amp;J16</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44</v>
-      </c>
-      <c r="X16" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64</v>
       </c>
       <c r="Y16" t="str">
         <f>Y15&amp;", "&amp;K16</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64</v>
+      </c>
+      <c r="Z16" t="str">
+        <f>Z15&amp;", "&amp;L16</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46</v>
       </c>
-      <c r="AA16" t="str">
-        <f>AA15&amp;", "&amp;M16</f>
+      <c r="AB16" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>90</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>42</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>43</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>65</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>45</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>63</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>45</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>13</v>
       </c>
-      <c r="O17" t="str">
-        <f t="shared" si="10"/>
+      <c r="P17" t="str">
+        <f>P16&amp;", "&amp;A18</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80</v>
       </c>
-      <c r="S17" t="str">
-        <f t="shared" si="4"/>
+      <c r="T17" t="str">
+        <f>T16&amp;", "&amp;F17</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42</v>
       </c>
-      <c r="T17" t="str">
-        <f t="shared" si="5"/>
+      <c r="U17" t="str">
+        <f>U16&amp;", "&amp;G17</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43</v>
       </c>
-      <c r="V17" t="str">
-        <f t="shared" si="6"/>
+      <c r="W17" t="str">
+        <f>W16&amp;", "&amp;I17</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65</v>
       </c>
-      <c r="W17" t="str">
-        <f t="shared" si="7"/>
+      <c r="X17" t="str">
+        <f>X16&amp;", "&amp;J17</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45</v>
-      </c>
-      <c r="X17" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64, 63</v>
       </c>
       <c r="Y17" t="str">
         <f>Y16&amp;", "&amp;K17</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64, 63</v>
+      </c>
+      <c r="Z17" t="str">
+        <f>Z16&amp;", "&amp;L17</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45</v>
       </c>
-      <c r="AA17" t="str">
-        <f>AA16&amp;", "&amp;M17</f>
+      <c r="AB17" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>90</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>44</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>64</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>46</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>41</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>44</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>14</v>
       </c>
-      <c r="O18" t="str">
-        <f t="shared" si="10"/>
+      <c r="P18" t="str">
+        <f>P17&amp;", "&amp;A19</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66</v>
       </c>
-      <c r="S18" t="str">
-        <f t="shared" si="4"/>
+      <c r="T18" t="str">
+        <f>T17&amp;", "&amp;F18</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90</v>
       </c>
-      <c r="T18" t="str">
-        <f t="shared" si="5"/>
+      <c r="U18" t="str">
+        <f>U17&amp;", "&amp;G18</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43, 44</v>
       </c>
-      <c r="V18" t="str">
-        <f t="shared" si="6"/>
+      <c r="W18" t="str">
+        <f>W17&amp;", "&amp;I18</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65, 64</v>
       </c>
-      <c r="W18" t="str">
-        <f t="shared" si="7"/>
+      <c r="X18" t="str">
+        <f>X17&amp;", "&amp;J18</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46</v>
-      </c>
-      <c r="X18" t="str">
-        <f t="shared" si="8"/>
-        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64, 63, 41</v>
       </c>
       <c r="Y18" t="str">
         <f>Y17&amp;", "&amp;K18</f>
+        <v>const char ltr_1[16] = { -15, 53, 54, 55, 32, 56, 72, 84, 92, 88, 78, 47, 65, 64, 63, 41</v>
+      </c>
+      <c r="Z18" t="str">
+        <f>Z17&amp;", "&amp;L18</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44</v>
       </c>
-      <c r="AA18" t="str">
-        <f>AA17&amp;", "&amp;M18</f>
+      <c r="AB18" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>66</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>92</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>45</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>63</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>47</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>43</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>15</v>
       </c>
-      <c r="O19" t="str">
-        <f t="shared" si="10"/>
+      <c r="P19" t="str">
+        <f>P18&amp;", "&amp;A20</f>
         <v>const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66, 46</v>
       </c>
-      <c r="S19" t="str">
-        <f t="shared" si="4"/>
+      <c r="T19" t="str">
+        <f>T18&amp;", "&amp;F19</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90, 92</v>
       </c>
-      <c r="T19" t="str">
-        <f t="shared" si="5"/>
+      <c r="U19" t="str">
+        <f>U18&amp;", "&amp;G19</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43, 44, 45</v>
       </c>
-      <c r="V19" t="str">
-        <f t="shared" si="6"/>
+      <c r="W19" t="str">
+        <f>W18&amp;", "&amp;I19</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65, 64, 63</v>
       </c>
-      <c r="W19" t="str">
-        <f t="shared" si="7"/>
+      <c r="X19" t="str">
+        <f>X18&amp;", "&amp;J19</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47</v>
       </c>
-      <c r="Y19" t="str">
-        <f>Y18&amp;", "&amp;K19</f>
+      <c r="Z19" t="str">
+        <f>Z18&amp;", "&amp;L19</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43</v>
       </c>
-      <c r="AA19" t="str">
-        <f>AA18&amp;", "&amp;M19</f>
+      <c r="AB19" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AE19">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>46</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>86</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>46</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>41</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>48</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>42</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>16</v>
       </c>
-      <c r="O20" t="str">
-        <f t="shared" si="10"/>
+      <c r="P20" t="str">
+        <f>P19&amp;", "&amp;A21</f>
         <v xml:space="preserve">const char ltr_P[18] = { -17, 81, 82, 70, 54, 55, 32, 33, 34, 59, 75, 86, 92, 90, 80, 66, 46, </v>
       </c>
-      <c r="S20" t="str">
-        <f t="shared" si="4"/>
+      <c r="T20" t="str">
+        <f>T19&amp;", "&amp;F20</f>
         <v>const char ltr_H[18] = { -17, 54, 70, 82, 81, 80, 66, 46, 34, 58, 74, 75, 76, 62, 42, 90, 92, 86</v>
       </c>
-      <c r="T20" t="str">
-        <f t="shared" si="5"/>
+      <c r="U20" t="str">
+        <f>U19&amp;", "&amp;G20</f>
         <v>const char ltr_S[18] = { -17, 34, 33, 32, 55, 54, 70, 82, 91, 92, 87, 76, 62, 42, 43, 44, 45, 46</v>
       </c>
-      <c r="V20" t="str">
-        <f t="shared" si="6"/>
+      <c r="W20" t="str">
+        <f>W19&amp;", "&amp;I20</f>
         <v>const char ltr_2[18] = { -17, 53, 54, 55, 32, 33, 34, 35, 58, 85, 92, 89, 66, 47, 65, 64, 63, 41</v>
       </c>
-      <c r="W20" t="str">
-        <f t="shared" si="7"/>
+      <c r="X20" t="str">
+        <f>X19&amp;", "&amp;J20</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48</v>
       </c>
-      <c r="Y20" t="str">
-        <f>Y19&amp;", "&amp;K20</f>
+      <c r="Z20" t="str">
+        <f>Z19&amp;", "&amp;L20</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42</v>
       </c>
-      <c r="AA20" t="str">
-        <f>AA19&amp;", "&amp;M20</f>
+      <c r="AB20" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I21">
+      <c r="AE20">
         <v>49</v>
       </c>
-      <c r="K21">
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>49</v>
+      </c>
+      <c r="L21">
         <v>62</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>17</v>
       </c>
-      <c r="W21" t="str">
-        <f t="shared" si="7"/>
+      <c r="X21" t="str">
+        <f>X20&amp;", "&amp;J21</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49</v>
       </c>
-      <c r="Y21" t="str">
-        <f>Y20&amp;", "&amp;K21</f>
+      <c r="Z21" t="str">
+        <f>Z20&amp;", "&amp;L21</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62</v>
       </c>
-      <c r="AA21" t="str">
-        <f>AA20&amp;", "&amp;M21</f>
+      <c r="AB21" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I22">
+      <c r="AE21">
         <v>50</v>
       </c>
-      <c r="K22">
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>50</v>
+      </c>
+      <c r="L22">
         <v>76</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>18</v>
       </c>
-      <c r="W22" t="str">
-        <f t="shared" si="7"/>
+      <c r="X22" t="str">
+        <f>X21&amp;", "&amp;J22</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50</v>
       </c>
-      <c r="Y22" t="str">
-        <f>Y21&amp;", "&amp;K22</f>
+      <c r="Z22" t="str">
+        <f>Z21&amp;", "&amp;L22</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76</v>
       </c>
-      <c r="AA22" t="str">
-        <f>AA21&amp;", "&amp;M22</f>
+      <c r="AB22" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I23">
+      <c r="AE22">
         <v>51</v>
       </c>
-      <c r="K23">
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>51</v>
+      </c>
+      <c r="L23">
         <v>87</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>19</v>
       </c>
-      <c r="W23" t="str">
-        <f t="shared" si="7"/>
+      <c r="X23" t="str">
+        <f>X22&amp;", "&amp;J23</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51</v>
       </c>
-      <c r="Y23" t="str">
-        <f>Y22&amp;", "&amp;K23</f>
+      <c r="Z23" t="str">
+        <f>Z22&amp;", "&amp;L23</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87</v>
       </c>
-      <c r="AA23" t="str">
-        <f>AA22&amp;", "&amp;M23</f>
+      <c r="AB23" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I24">
+      <c r="AE23">
         <v>52</v>
       </c>
-      <c r="K24">
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>52</v>
+      </c>
+      <c r="L24">
         <v>91</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>20</v>
       </c>
-      <c r="W24" t="str">
-        <f t="shared" si="7"/>
+      <c r="X24" t="str">
+        <f>X23&amp;", "&amp;J24</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52</v>
       </c>
-      <c r="Y24" t="str">
-        <f>Y23&amp;", "&amp;K24</f>
+      <c r="Z24" t="str">
+        <f>Z23&amp;", "&amp;L24</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91</v>
       </c>
-      <c r="AA24" t="str">
-        <f>AA23&amp;", "&amp;M24</f>
+      <c r="AB24" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I25">
+      <c r="AE24">
         <v>53</v>
       </c>
-      <c r="K25">
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>53</v>
+      </c>
+      <c r="L25">
         <v>82</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>21</v>
       </c>
-      <c r="W25" t="str">
-        <f t="shared" si="7"/>
+      <c r="X25" t="str">
+        <f>X24&amp;", "&amp;J25</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53</v>
       </c>
-      <c r="Y25" t="str">
-        <f>Y24&amp;", "&amp;K25</f>
+      <c r="Z25" t="str">
+        <f>Z24&amp;", "&amp;L25</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91, 82</v>
       </c>
-      <c r="AA25" t="str">
-        <f>AA24&amp;", "&amp;M25</f>
+      <c r="AB25" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I26">
+      <c r="AE25">
         <v>54</v>
       </c>
-      <c r="K26">
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>54</v>
+      </c>
+      <c r="L26">
         <v>70</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>22</v>
       </c>
-      <c r="W26" t="str">
-        <f t="shared" si="7"/>
+      <c r="X26" t="str">
+        <f>X25&amp;", "&amp;J26</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54</v>
       </c>
-      <c r="Y26" t="str">
-        <f>Y25&amp;", "&amp;K26</f>
+      <c r="Z26" t="str">
+        <f>Z25&amp;", "&amp;L26</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91, 82, 70</v>
       </c>
-      <c r="AA26" t="str">
-        <f>AA25&amp;", "&amp;M26</f>
+      <c r="AB26" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I27">
+      <c r="AE26">
         <v>55</v>
       </c>
-      <c r="K27">
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>55</v>
+      </c>
+      <c r="L27">
         <v>54</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>23</v>
       </c>
-      <c r="W27" t="str">
-        <f t="shared" si="7"/>
+      <c r="X27" t="str">
+        <f>X26&amp;", "&amp;J27</f>
         <v>const char ltr_0[25] = { -24, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55</v>
       </c>
-      <c r="Y27" t="str">
-        <f>Y26&amp;", "&amp;K27</f>
+      <c r="Z27" t="str">
+        <f>Z26&amp;", "&amp;L27</f>
         <v>const char ltr_8[25] = { -24, 54, 55, 32, 33, 34, 58, 74, 85, 92, 89, 80, 66, 46, 45, 44, 43, 42, 62, 76, 87, 91, 82, 70, 54</v>
       </c>
-      <c r="AA27" t="str">
-        <f>AA26&amp;", "&amp;M27</f>
+      <c r="AB27" t="str">
+        <f t="shared" si="1"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M28">
+      <c r="AE27">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N28">
         <v>24</v>
       </c>
-      <c r="AA28" t="str">
-        <f t="shared" ref="AA28:AA91" si="11">AA27&amp;", "&amp;M28</f>
+      <c r="AB28" t="str">
+        <f t="shared" ref="AB28:AB91" si="2">AB27&amp;", "&amp;N28</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M29">
+      <c r="AE28">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N29">
         <v>25</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>176</v>
       </c>
-      <c r="AA29" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB29" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M30">
+      <c r="AE29">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N30">
         <v>26</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>177</v>
       </c>
-      <c r="AA30" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB30" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M31">
+      <c r="AE30">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N31">
         <v>27</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>178</v>
       </c>
-      <c r="AA31" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB31" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="M32">
+      <c r="AE31">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N32">
         <v>28</v>
       </c>
-      <c r="AA32" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB32" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28</v>
       </c>
-    </row>
-    <row r="33" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M33">
+      <c r="AE32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N33">
         <v>29</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>163</v>
       </c>
-      <c r="AA33" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB33" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29</v>
       </c>
-    </row>
-    <row r="34" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M34">
+      <c r="AE33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N34">
         <v>30</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>156</v>
       </c>
-      <c r="AA34" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB34" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30</v>
       </c>
-    </row>
-    <row r="35" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M35">
+      <c r="AE34">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N35">
         <v>31</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>157</v>
       </c>
-      <c r="AA35" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB35" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31</v>
       </c>
-    </row>
-    <row r="36" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M36">
+      <c r="AE35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N36">
         <v>32</v>
       </c>
-      <c r="AA36" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB36" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32</v>
       </c>
-    </row>
-    <row r="37" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M37">
+      <c r="AE36">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N37">
         <v>33</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>158</v>
       </c>
-      <c r="AA37" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB37" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33</v>
       </c>
-    </row>
-    <row r="38" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M38">
+      <c r="AE37">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N38">
         <v>34</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>159</v>
       </c>
-      <c r="AA38" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB38" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34</v>
       </c>
-    </row>
-    <row r="39" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M39">
+      <c r="AE38">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N39">
         <v>35</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>160</v>
       </c>
-      <c r="AA39" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB39" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35</v>
       </c>
-    </row>
-    <row r="40" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M40">
+      <c r="AE39">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N40">
         <v>36</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>161</v>
       </c>
-      <c r="AA40" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB40" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36</v>
       </c>
-    </row>
-    <row r="41" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M41">
+      <c r="AE40">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N41">
         <v>37</v>
       </c>
-      <c r="AA41" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB41" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37</v>
       </c>
-    </row>
-    <row r="42" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M42">
+      <c r="AE41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N42">
         <v>38</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>162</v>
       </c>
-      <c r="AA42" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB42" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38</v>
       </c>
-    </row>
-    <row r="43" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M43">
+      <c r="AE42">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N43">
         <v>39</v>
       </c>
-      <c r="AA43" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB43" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39</v>
       </c>
-    </row>
-    <row r="44" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M44">
+      <c r="AE43">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N44">
         <v>40</v>
       </c>
-      <c r="AA44" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB44" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40</v>
       </c>
-    </row>
-    <row r="45" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M45">
+      <c r="AE44">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N45">
         <v>41</v>
       </c>
-      <c r="AA45" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB45" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41</v>
       </c>
-    </row>
-    <row r="46" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M46">
+      <c r="AE45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N46">
         <v>42</v>
       </c>
-      <c r="AA46" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB46" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42</v>
       </c>
-    </row>
-    <row r="47" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M47">
+      <c r="AE46">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N47">
         <v>43</v>
       </c>
-      <c r="AA47" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB47" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43</v>
       </c>
-    </row>
-    <row r="48" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M48">
+      <c r="AE47">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N48">
         <v>44</v>
       </c>
-      <c r="AA48" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB48" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44</v>
       </c>
-    </row>
-    <row r="49" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M49">
+      <c r="AE48">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N49">
         <v>45</v>
       </c>
-      <c r="AA49" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB49" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45</v>
       </c>
-    </row>
-    <row r="50" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M50">
+      <c r="AE49">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N50">
         <v>46</v>
       </c>
-      <c r="AA50" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB50" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46</v>
       </c>
-    </row>
-    <row r="51" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M51">
+      <c r="AE50">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N51">
         <v>47</v>
       </c>
-      <c r="AA51" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB51" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47</v>
       </c>
-    </row>
-    <row r="52" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M52">
+      <c r="AE51">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N52">
         <v>48</v>
       </c>
-      <c r="AA52" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB52" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48</v>
       </c>
-    </row>
-    <row r="53" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M53">
+      <c r="AE52">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N53">
         <v>49</v>
       </c>
-      <c r="AA53" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB53" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49</v>
       </c>
     </row>
-    <row r="54" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M54">
+    <row r="54" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N54">
         <v>50</v>
       </c>
-      <c r="AA54" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB54" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50</v>
       </c>
     </row>
-    <row r="55" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M55">
+    <row r="55" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N55">
         <v>51</v>
       </c>
-      <c r="AA55" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB55" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51</v>
       </c>
     </row>
-    <row r="56" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M56">
+    <row r="56" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N56">
         <v>52</v>
       </c>
-      <c r="AA56" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB56" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52</v>
       </c>
     </row>
-    <row r="57" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M57">
+    <row r="57" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N57">
         <v>53</v>
       </c>
-      <c r="AA57" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB57" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53</v>
       </c>
     </row>
-    <row r="58" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M58">
+    <row r="58" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N58">
         <v>54</v>
       </c>
-      <c r="AA58" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB58" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54</v>
       </c>
     </row>
-    <row r="59" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M59">
+    <row r="59" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N59">
         <v>55</v>
       </c>
-      <c r="AA59" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB59" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55</v>
       </c>
     </row>
-    <row r="60" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M60">
+    <row r="60" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N60">
         <v>56</v>
       </c>
-      <c r="AA60" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB60" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56</v>
       </c>
     </row>
-    <row r="61" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M61">
+    <row r="61" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N61">
         <v>57</v>
       </c>
-      <c r="AA61" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB61" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57</v>
       </c>
     </row>
-    <row r="62" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M62">
+    <row r="62" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N62">
         <v>58</v>
       </c>
-      <c r="AA62" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB62" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58</v>
       </c>
     </row>
-    <row r="63" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M63">
+    <row r="63" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N63">
         <v>59</v>
       </c>
-      <c r="AA63" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB63" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59</v>
       </c>
     </row>
-    <row r="64" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M64">
+    <row r="64" spans="14:31" x14ac:dyDescent="0.25">
+      <c r="N64">
         <v>60</v>
       </c>
-      <c r="AA64" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB64" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60</v>
       </c>
     </row>
-    <row r="65" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M65">
+    <row r="65" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N65">
         <v>61</v>
       </c>
-      <c r="AA65" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB65" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61</v>
       </c>
     </row>
-    <row r="66" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M66">
+    <row r="66" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N66">
         <v>62</v>
       </c>
-      <c r="AA66" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB66" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62</v>
       </c>
     </row>
-    <row r="67" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M67">
+    <row r="67" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N67">
         <v>63</v>
       </c>
-      <c r="AA67" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB67" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63</v>
       </c>
     </row>
-    <row r="68" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M68">
+    <row r="68" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N68">
         <v>64</v>
       </c>
-      <c r="AA68" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB68" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64</v>
       </c>
     </row>
-    <row r="69" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M69">
+    <row r="69" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N69">
         <v>65</v>
       </c>
-      <c r="AA69" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB69" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65</v>
       </c>
     </row>
-    <row r="70" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M70">
+    <row r="70" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N70">
         <v>66</v>
       </c>
-      <c r="AA70" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB70" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66</v>
       </c>
     </row>
-    <row r="71" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M71">
+    <row r="71" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N71">
         <v>67</v>
       </c>
-      <c r="AA71" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB71" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67</v>
       </c>
     </row>
-    <row r="72" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M72">
+    <row r="72" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N72">
         <v>68</v>
       </c>
-      <c r="AA72" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB72" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68</v>
       </c>
     </row>
-    <row r="73" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M73">
+    <row r="73" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N73">
         <v>69</v>
       </c>
-      <c r="AA73" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB73" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69</v>
       </c>
     </row>
-    <row r="74" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M74">
+    <row r="74" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N74">
         <v>70</v>
       </c>
-      <c r="AA74" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB74" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70</v>
       </c>
     </row>
-    <row r="75" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M75">
+    <row r="75" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N75">
         <v>71</v>
       </c>
-      <c r="AA75" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB75" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71</v>
       </c>
     </row>
-    <row r="76" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M76">
+    <row r="76" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N76">
         <v>72</v>
       </c>
-      <c r="AA76" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB76" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72</v>
       </c>
     </row>
-    <row r="77" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M77">
+    <row r="77" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N77">
         <v>73</v>
       </c>
-      <c r="AA77" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB77" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73</v>
       </c>
     </row>
-    <row r="78" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M78">
+    <row r="78" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N78">
         <v>74</v>
       </c>
-      <c r="AA78" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB78" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74</v>
       </c>
     </row>
-    <row r="79" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M79">
+    <row r="79" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N79">
         <v>75</v>
       </c>
-      <c r="AA79" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB79" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75</v>
       </c>
     </row>
-    <row r="80" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M80">
+    <row r="80" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N80">
         <v>76</v>
       </c>
-      <c r="AA80" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB80" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76</v>
       </c>
     </row>
-    <row r="81" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M81">
+    <row r="81" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N81">
         <v>77</v>
       </c>
-      <c r="AA81" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB81" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77</v>
       </c>
     </row>
-    <row r="82" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M82">
+    <row r="82" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N82">
         <v>78</v>
       </c>
-      <c r="AA82" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB82" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78</v>
       </c>
     </row>
-    <row r="83" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M83">
+    <row r="83" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N83">
         <v>79</v>
       </c>
-      <c r="AA83" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB83" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79</v>
       </c>
     </row>
-    <row r="84" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M84">
+    <row r="84" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N84">
         <v>80</v>
       </c>
-      <c r="AA84" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB84" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80</v>
       </c>
     </row>
-    <row r="85" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M85">
+    <row r="85" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N85">
         <v>81</v>
       </c>
-      <c r="AA85" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB85" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81</v>
       </c>
     </row>
-    <row r="86" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M86">
+    <row r="86" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N86">
         <v>82</v>
       </c>
-      <c r="AA86" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB86" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82</v>
       </c>
     </row>
-    <row r="87" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M87">
+    <row r="87" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N87">
         <v>83</v>
       </c>
-      <c r="AA87" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB87" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83</v>
       </c>
     </row>
-    <row r="88" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M88">
+    <row r="88" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N88">
         <v>84</v>
       </c>
-      <c r="AA88" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB88" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84</v>
       </c>
     </row>
-    <row r="89" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M89">
+    <row r="89" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N89">
         <v>85</v>
       </c>
-      <c r="AA89" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB89" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85</v>
       </c>
     </row>
-    <row r="90" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M90">
+    <row r="90" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N90">
         <v>86</v>
       </c>
-      <c r="AA90" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB90" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86</v>
       </c>
     </row>
-    <row r="91" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M91">
+    <row r="91" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N91">
         <v>87</v>
       </c>
-      <c r="AA91" t="str">
-        <f t="shared" si="11"/>
+      <c r="AB91" t="str">
+        <f t="shared" si="2"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87</v>
       </c>
     </row>
-    <row r="92" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M92">
+    <row r="92" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N92">
         <v>88</v>
       </c>
-      <c r="AA92" t="str">
-        <f t="shared" ref="AA92:AA96" si="12">AA91&amp;", "&amp;M92</f>
+      <c r="AB92" t="str">
+        <f t="shared" ref="AB92:AB96" si="3">AB91&amp;", "&amp;N92</f>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88</v>
       </c>
     </row>
-    <row r="93" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M93">
+    <row r="93" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N93">
         <v>89</v>
       </c>
-      <c r="AA93" t="str">
-        <f t="shared" si="12"/>
+      <c r="AB93" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89</v>
       </c>
     </row>
-    <row r="94" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M94">
+    <row r="94" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N94">
         <v>90</v>
       </c>
-      <c r="AA94" t="str">
-        <f t="shared" si="12"/>
+      <c r="AB94" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90</v>
       </c>
     </row>
-    <row r="95" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M95">
+    <row r="95" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N95">
         <v>91</v>
       </c>
-      <c r="AA95" t="str">
-        <f t="shared" si="12"/>
+      <c r="AB95" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91</v>
       </c>
     </row>
-    <row r="96" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M96">
+    <row r="96" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N96">
         <v>92</v>
       </c>
-      <c r="AA96" t="str">
-        <f t="shared" si="12"/>
+      <c r="AB96" t="str">
+        <f t="shared" si="3"/>
         <v>const char ltr_all[94] = { -93, 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A21:A35">
-    <sortCondition ref="A20"/>
+  <sortState ref="AE3:AE121">
+    <sortCondition ref="AE3:AE121"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>